<commit_message>
improved balancing of carbon sankey
</commit_message>
<xml_diff>
--- a/SEPIA/SEPIA_config.xlsx
+++ b/SEPIA/SEPIA_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" state="visible" r:id="rId2"/>
@@ -447,7 +447,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="1075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2048" uniqueCount="1077">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -3185,6 +3185,9 @@
     <t xml:space="preserve">emmserbmmatm</t>
   </si>
   <si>
+    <t xml:space="preserve">oil</t>
+  </si>
+  <si>
     <t xml:space="preserve">oil emissions</t>
   </si>
   <si>
@@ -3225,6 +3228,9 @@
   </si>
   <si>
     <t xml:space="preserve">emmfossoil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">net</t>
   </si>
   <si>
     <t xml:space="preserve">Net Emissions</t>
@@ -5710,10 +5716,10 @@
   <dimension ref="A1:T95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D53" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
       <selection pane="bottomRight" activeCell="J59" activeCellId="0" sqref="J59"/>
     </sheetView>
   </sheetViews>
@@ -8136,8 +8142,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A112" activeCellId="0" sqref="A112"/>
     </sheetView>
@@ -13798,9 +13804,9 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A50" activeCellId="0" sqref="A50"/>
+      <selection pane="bottomLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14337,12 +14343,14 @@
       <c r="B31" s="25" t="s">
         <v>325</v>
       </c>
-      <c r="C31" s="41"/>
+      <c r="C31" s="41" t="s">
+        <v>912</v>
+      </c>
       <c r="D31" s="43" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="E31" s="43" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="F31" s="41"/>
       <c r="G31" s="41"/>
@@ -14356,10 +14364,10 @@
       </c>
       <c r="C32" s="41"/>
       <c r="D32" s="43" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="E32" s="43" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="F32" s="41"/>
       <c r="G32" s="41"/>
@@ -14373,10 +14381,10 @@
       </c>
       <c r="C33" s="41"/>
       <c r="D33" s="43" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="E33" s="43" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="F33" s="41"/>
       <c r="G33" s="41"/>
@@ -14390,10 +14398,10 @@
       </c>
       <c r="C34" s="41"/>
       <c r="D34" s="43" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="F34" s="41"/>
       <c r="G34" s="41"/>
@@ -14407,10 +14415,10 @@
       </c>
       <c r="C35" s="41"/>
       <c r="D35" s="43" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F35" s="41"/>
       <c r="G35" s="41"/>
@@ -14427,7 +14435,7 @@
         <v>342</v>
       </c>
       <c r="E36" s="43" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="F36" s="41"/>
       <c r="G36" s="41"/>
@@ -14441,10 +14449,10 @@
       </c>
       <c r="C37" s="41"/>
       <c r="D37" s="43" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="F37" s="41"/>
       <c r="G37" s="41"/>
@@ -14461,7 +14469,7 @@
         <v>823</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="F38" s="41"/>
       <c r="G38" s="41"/>
@@ -14473,12 +14481,14 @@
       <c r="B39" s="25" t="s">
         <v>347</v>
       </c>
-      <c r="C39" s="41"/>
+      <c r="C39" s="41" t="s">
+        <v>927</v>
+      </c>
       <c r="D39" s="43" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="E39" s="43" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="F39" s="41"/>
       <c r="G39" s="41"/>
@@ -14492,10 +14502,10 @@
       </c>
       <c r="C40" s="41"/>
       <c r="D40" s="43" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="E40" s="43" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="F40" s="41"/>
       <c r="G40" s="41"/>
@@ -14509,10 +14519,10 @@
       </c>
       <c r="C41" s="41"/>
       <c r="D41" s="43" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="F41" s="41"/>
       <c r="G41" s="41"/>
@@ -14526,10 +14536,10 @@
       </c>
       <c r="C42" s="41"/>
       <c r="D42" s="43" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="E42" s="43" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="F42" s="41"/>
       <c r="G42" s="41"/>
@@ -14543,10 +14553,10 @@
       </c>
       <c r="C43" s="41"/>
       <c r="D43" s="43" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="E43" s="43" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="F43" s="41"/>
       <c r="G43" s="41"/>
@@ -14563,7 +14573,7 @@
         <v>350</v>
       </c>
       <c r="E44" s="43" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="F44" s="41"/>
       <c r="G44" s="41"/>
@@ -14577,10 +14587,10 @@
       </c>
       <c r="C45" s="41"/>
       <c r="D45" s="43" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="E45" s="43" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="F45" s="41"/>
       <c r="G45" s="41"/>
@@ -14594,10 +14604,10 @@
       </c>
       <c r="C46" s="41"/>
       <c r="D46" s="43" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="E46" s="43" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="F46" s="41"/>
       <c r="G46" s="41"/>
@@ -14611,10 +14621,10 @@
       </c>
       <c r="C47" s="41"/>
       <c r="D47" s="43" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="E47" s="43" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="F47" s="41"/>
       <c r="G47" s="41"/>
@@ -14628,10 +14638,10 @@
       </c>
       <c r="C48" s="41"/>
       <c r="D48" s="43" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="E48" s="49" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="F48" s="41"/>
       <c r="G48" s="41"/>
@@ -14645,10 +14655,10 @@
       </c>
       <c r="C49" s="41"/>
       <c r="D49" s="43" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="E49" s="49" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="F49" s="41"/>
       <c r="G49" s="41"/>
@@ -14665,7 +14675,7 @@
         <v>352</v>
       </c>
       <c r="E50" s="49" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="F50" s="41"/>
       <c r="G50" s="41"/>
@@ -14682,7 +14692,7 @@
         <v>352</v>
       </c>
       <c r="E51" s="49" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="F51" s="41"/>
       <c r="G51" s="41"/>
@@ -14696,10 +14706,10 @@
       </c>
       <c r="C52" s="41"/>
       <c r="D52" s="43" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="E52" s="49" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="F52" s="41"/>
       <c r="G52" s="41"/>
@@ -14716,7 +14726,7 @@
         <v>487</v>
       </c>
       <c r="E53" s="49" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="F53" s="41"/>
       <c r="G53" s="41"/>
@@ -14968,10 +14978,10 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="bottomLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15068,7 +15078,7 @@
       </c>
       <c r="C5" s="41"/>
       <c r="D5" s="43" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="E5" s="43" t="s">
         <v>869</v>
@@ -15095,7 +15105,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="47" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>220</v>
@@ -15112,7 +15122,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="47" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>220</v>
@@ -15129,7 +15139,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="47" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>220</v>
@@ -15146,7 +15156,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="47" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>220</v>
@@ -15163,7 +15173,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="47" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>220</v>
@@ -15197,7 +15207,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="47" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>218</v>
@@ -15214,7 +15224,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="47" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>218</v>
@@ -15231,7 +15241,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="47" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>218</v>
@@ -15248,7 +15258,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="47" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>218</v>
@@ -15265,7 +15275,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="47" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>220</v>
@@ -15282,85 +15292,87 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="47" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="C18" s="41"/>
+      <c r="C18" s="41" t="s">
+        <v>912</v>
+      </c>
       <c r="D18" s="43" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="E18" s="43" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="F18" s="41"/>
       <c r="G18" s="41"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="47" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>218</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="43" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="E19" s="43" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="F19" s="41"/>
       <c r="G19" s="41"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="47" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>218</v>
       </c>
       <c r="C20" s="41"/>
       <c r="D20" s="43" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="E20" s="43" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="F20" s="41"/>
       <c r="G20" s="41"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="47" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>218</v>
       </c>
       <c r="C21" s="41"/>
       <c r="D21" s="43" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="F21" s="41"/>
       <c r="G21" s="41"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="47" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>230</v>
       </c>
       <c r="C22" s="41"/>
       <c r="D22" s="43" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="F22" s="41"/>
       <c r="G22" s="41"/>
@@ -15377,24 +15389,24 @@
         <v>342</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="F23" s="41"/>
       <c r="G23" s="41"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="47" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="B24" s="25" t="s">
         <v>220</v>
       </c>
       <c r="C24" s="41"/>
       <c r="D24" s="43" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="E24" s="43" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
@@ -15408,10 +15420,10 @@
       </c>
       <c r="C25" s="41"/>
       <c r="D25" s="43" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="E25" s="43" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
@@ -15425,10 +15437,10 @@
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="43" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
@@ -15445,7 +15457,7 @@
         <v>352</v>
       </c>
       <c r="E27" s="49" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
@@ -15758,563 +15770,563 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="C2" s="51" t="s">
+        <v>959</v>
+      </c>
+      <c r="D2" s="52" t="s">
         <v>957</v>
       </c>
-      <c r="D2" s="52" t="s">
-        <v>955</v>
-      </c>
       <c r="E2" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B3" s="50" t="s">
+        <v>962</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>963</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>961</v>
+      </c>
+      <c r="E3" s="53" t="s">
         <v>960</v>
-      </c>
-      <c r="C3" s="51" t="s">
-        <v>961</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>959</v>
-      </c>
-      <c r="E3" s="53" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="C4" s="51" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="C5" s="51" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="C8" s="51" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D8" s="52" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D9" s="52" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="C12" s="51" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D12" s="52" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="C13" s="54" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D13" s="52" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="B14" s="50" t="s">
+        <v>986</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>963</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>985</v>
+      </c>
+      <c r="E14" s="55" t="s">
         <v>984</v>
-      </c>
-      <c r="C14" s="54" t="s">
-        <v>961</v>
-      </c>
-      <c r="D14" s="52" t="s">
-        <v>983</v>
-      </c>
-      <c r="E14" s="55" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D15" s="52" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="C16" s="54" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D16" s="52" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="C17" s="54" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D17" s="52" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="E17" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D18" s="52" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="E18" s="53" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="B19" s="56" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D19" s="52" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B20" s="50" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="D20" s="52" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E20" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B21" s="57" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="C21" s="51" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D21" s="52" t="s">
         <v>1001</v>
       </c>
-      <c r="D21" s="52" t="s">
-        <v>999</v>
-      </c>
       <c r="E21" s="53" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B22" s="58" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C22" s="51" t="s">
         <v>1003</v>
       </c>
-      <c r="B22" s="58" t="s">
-        <v>1004</v>
-      </c>
-      <c r="C22" s="51" t="s">
-        <v>1001</v>
-      </c>
       <c r="D22" s="52" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E22" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B23" s="50" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="D23" s="52" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="E23" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B24" s="50" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="D24" s="52" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="E24" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="B25" s="50" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="C25" s="51" t="s">
+        <v>1014</v>
+      </c>
+      <c r="D25" s="52" t="s">
         <v>1012</v>
       </c>
-      <c r="D25" s="52" t="s">
-        <v>1010</v>
-      </c>
       <c r="E25" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="B26" s="59" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="D26" s="60" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="E26" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B27" s="59" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="C27" s="61" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="D27" s="60" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="E27" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B28" s="59" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="C28" s="61" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="D28" s="60" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="E28" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="B29" s="59" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="C29" s="61" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="D29" s="60" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="E29" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="B30" s="59" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="D30" s="60" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="E30" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="B31" s="59" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="C31" s="61" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="D31" s="60" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="E31" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="B32" s="50" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="D32" s="52" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="E32" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="B33" s="56" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="C33" s="54" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D33" s="60" t="s">
         <v>1035</v>
       </c>
-      <c r="D33" s="60" t="s">
-        <v>1033</v>
-      </c>
       <c r="E33" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="B34" s="56" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C34" s="54" t="s">
         <v>1037</v>
       </c>
-      <c r="C34" s="54" t="s">
-        <v>1035</v>
-      </c>
       <c r="D34" s="52" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="E34" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
   </sheetData>
@@ -16375,274 +16387,274 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="C2" s="51"/>
       <c r="D2" s="52" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="E2" s="62" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="C3" s="51" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D3" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="D3" s="52" t="s">
-        <v>1040</v>
-      </c>
       <c r="E3" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="B4" s="50" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="C4" s="51"/>
       <c r="D4" s="52" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="B5" s="50" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="C5" s="51"/>
       <c r="D5" s="52" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="B6" s="50" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="C6" s="51"/>
       <c r="D6" s="52" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="B7" s="50" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="C7" s="51"/>
       <c r="D7" s="52" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="E7" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="B8" s="50" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="C8" s="51"/>
       <c r="D8" s="52" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="C9" s="51"/>
       <c r="D9" s="52" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="B10" s="50" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="C10" s="51"/>
       <c r="D10" s="52" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="B11" s="50" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="C11" s="51"/>
       <c r="D11" s="52" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="B12" s="50" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="C12" s="51"/>
       <c r="D12" s="52" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="C13" s="51"/>
       <c r="D13" s="52" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="E13" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="C14" s="51"/>
       <c r="D14" s="52" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="E14" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="B15" s="50" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="C15" s="51"/>
       <c r="D15" s="52" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="E15" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="B16" s="50" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="C16" s="51"/>
       <c r="D16" s="52" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="B17" s="50" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="C17" s="51"/>
       <c r="D17" s="52" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="B18" s="50" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="C18" s="51"/>
       <c r="D18" s="52" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="C19" s="51"/>
       <c r="D19" s="52" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="E19" s="55" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NL lulucf correction + temporary FT correction
</commit_message>
<xml_diff>
--- a/SEPIA/SEPIA_config.xlsx
+++ b/SEPIA/SEPIA_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" state="visible" r:id="rId2"/>
@@ -447,7 +447,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="1084">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2069" uniqueCount="1086">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -3315,6 +3315,12 @@
   </si>
   <si>
     <t xml:space="preserve">emmimpmet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LULUCF Emmissions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emmlulucf</t>
   </si>
   <si>
     <t xml:space="preserve">OCGT emissions</t>
@@ -5756,11 +5762,11 @@
   </sheetPr>
   <dimension ref="A1:T96"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D65" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
       <selection pane="bottomRight" activeCell="C96" activeCellId="0" sqref="C96"/>
     </sheetView>
   </sheetViews>
@@ -13858,10 +13864,10 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
+      <selection pane="bottomLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14811,7 +14817,23 @@
       <c r="F54" s="42"/>
       <c r="G54" s="42"/>
     </row>
-    <row r="1048352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="48" t="s">
+        <v>341</v>
+      </c>
+      <c r="B55" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="C55" s="42"/>
+      <c r="D55" s="44" t="s">
+        <v>956</v>
+      </c>
+      <c r="E55" s="50" t="s">
+        <v>957</v>
+      </c>
+      <c r="F55" s="42"/>
+      <c r="G55" s="42"/>
+    </row>
     <row r="1048353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -15157,7 +15179,7 @@
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="44" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E5" s="44" t="s">
         <v>871</v>
@@ -15184,7 +15206,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="48" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>220</v>
@@ -15201,7 +15223,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="48" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B8" s="25" t="s">
         <v>220</v>
@@ -15218,7 +15240,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="48" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>220</v>
@@ -15235,7 +15257,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="48" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>220</v>
@@ -15252,7 +15274,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>220</v>
@@ -15286,7 +15308,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="48" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>218</v>
@@ -15303,7 +15325,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="48" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>218</v>
@@ -15320,7 +15342,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="48" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>218</v>
@@ -15337,7 +15359,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="48" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>218</v>
@@ -15354,7 +15376,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="48" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>220</v>
@@ -15371,7 +15393,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="48" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B18" s="25" t="s">
         <v>218</v>
@@ -15390,7 +15412,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="48" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>218</v>
@@ -15407,7 +15429,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="48" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>218</v>
@@ -15424,7 +15446,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="48" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>218</v>
@@ -15441,7 +15463,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="48" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>230</v>
@@ -15458,7 +15480,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="48" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>230</v>
@@ -15467,7 +15489,7 @@
         <v>953</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="E23" s="51" t="s">
         <v>955</v>
@@ -15494,7 +15516,7 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="48" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>220</v>
@@ -15867,563 +15889,563 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="C2" s="53" t="s">
+        <v>968</v>
+      </c>
+      <c r="D2" s="54" t="s">
         <v>966</v>
       </c>
-      <c r="D2" s="54" t="s">
-        <v>964</v>
-      </c>
       <c r="E2" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B3" s="52" t="s">
+        <v>971</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>972</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>970</v>
+      </c>
+      <c r="E3" s="55" t="s">
         <v>969</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>970</v>
-      </c>
-      <c r="D3" s="54" t="s">
-        <v>968</v>
-      </c>
-      <c r="E3" s="55" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="D4" s="54" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="C7" s="56" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="E7" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="B14" s="52" t="s">
+        <v>995</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>972</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>994</v>
+      </c>
+      <c r="E14" s="57" t="s">
         <v>993</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>970</v>
-      </c>
-      <c r="D14" s="54" t="s">
-        <v>992</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D15" s="54" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="C19" s="56" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="C20" s="53" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="D20" s="54" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="E20" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="C21" s="53" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D21" s="54" t="s">
         <v>1010</v>
       </c>
-      <c r="D21" s="54" t="s">
-        <v>1008</v>
-      </c>
       <c r="E21" s="55" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B22" s="60" t="s">
+        <v>1015</v>
+      </c>
+      <c r="C22" s="53" t="s">
         <v>1012</v>
       </c>
-      <c r="B22" s="60" t="s">
-        <v>1013</v>
-      </c>
-      <c r="C22" s="53" t="s">
-        <v>1010</v>
-      </c>
       <c r="D22" s="54" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E22" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="C23" s="53" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="E23" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C24" s="53" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D24" s="54" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="E24" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B25" s="52" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="C25" s="53" t="s">
+        <v>1023</v>
+      </c>
+      <c r="D25" s="54" t="s">
         <v>1021</v>
       </c>
-      <c r="D25" s="54" t="s">
-        <v>1019</v>
-      </c>
       <c r="E25" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="C26" s="53" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D26" s="62" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="E26" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D27" s="62" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="E27" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="B28" s="61" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D28" s="62" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="E28" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="B29" s="61" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="C29" s="63" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D29" s="62" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="E29" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="B30" s="61" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="C30" s="53" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D30" s="62" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="E30" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D31" s="62" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="E31" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="D32" s="54" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="E32" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="C33" s="56" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D33" s="62" t="s">
         <v>1044</v>
       </c>
-      <c r="D33" s="62" t="s">
-        <v>1042</v>
-      </c>
       <c r="E33" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="B34" s="58" t="s">
+        <v>1048</v>
+      </c>
+      <c r="C34" s="56" t="s">
         <v>1046</v>
       </c>
-      <c r="C34" s="56" t="s">
-        <v>1044</v>
-      </c>
       <c r="D34" s="54" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="E34" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
   </sheetData>
@@ -16484,274 +16506,274 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="54" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="C3" s="53" t="s">
+        <v>1053</v>
+      </c>
+      <c r="D3" s="54" t="s">
         <v>1051</v>
       </c>
-      <c r="D3" s="54" t="s">
-        <v>1049</v>
-      </c>
       <c r="E3" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="C4" s="53"/>
       <c r="D4" s="54" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="E4" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="C5" s="53"/>
       <c r="D5" s="54" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="E5" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="54" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="E6" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="54" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="E7" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="C8" s="53"/>
       <c r="D8" s="54" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="E8" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="C9" s="53"/>
       <c r="D9" s="54" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="E9" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C10" s="53"/>
       <c r="D10" s="54" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="C11" s="53"/>
       <c r="D11" s="54" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="E11" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="C12" s="53"/>
       <c r="D12" s="54" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="C13" s="53"/>
       <c r="D13" s="54" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="C14" s="53"/>
       <c r="D14" s="54" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="C15" s="53"/>
       <c r="D15" s="54" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="C16" s="53"/>
       <c r="D16" s="54" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="C17" s="53"/>
       <c r="D17" s="54" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="E17" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="C18" s="53"/>
       <c r="D18" s="54" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="E18" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="C19" s="53"/>
       <c r="D19" s="54" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
including rail freight demand and small corrections in esidential and tertiary demands
</commit_message>
<xml_diff>
--- a/SEPIA/SEPIA_config.xlsx
+++ b/SEPIA/SEPIA_config.xlsx
@@ -5145,7 +5145,7 @@
       <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.91"/>
@@ -5755,7 +5755,7 @@
       <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.28"/>
@@ -5938,7 +5938,7 @@
       <selection pane="bottomRight" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.36"/>
@@ -8469,12 +8469,12 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A280" activeCellId="0" sqref="A280"/>
+      <selection pane="bottomLeft" activeCell="A246" activeCellId="0" sqref="A246"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -13256,7 +13256,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="26" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
       <c r="B246" s="26" t="s">
         <v>132</v>
@@ -14254,7 +14254,7 @@
       <selection pane="bottomLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -15679,7 +15679,7 @@
       <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -16305,7 +16305,7 @@
       <selection pane="bottomLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -16922,7 +16922,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -17247,7 +17247,7 @@
       <selection pane="bottomRight" activeCell="AQ9" activeCellId="0" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.23828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.27"/>

</xml_diff>

<commit_message>
include total country results in sankey and excel generator
</commit_message>
<xml_diff>
--- a/SEPIA/SEPIA_config.xlsx
+++ b/SEPIA/SEPIA_config.xlsx
@@ -447,7 +447,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="1145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="1147">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -2687,6 +2687,9 @@
     <t xml:space="preserve">prespaccfres</t>
   </si>
   <si>
+    <t xml:space="preserve">Residential and tertiary HP sources for heating</t>
+  </si>
+  <si>
     <t xml:space="preserve">prespaccfra</t>
   </si>
   <si>
@@ -2697,6 +2700,9 @@
   </si>
   <si>
     <t xml:space="preserve">prespaccfta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential and tertiary HP for heating</t>
   </si>
   <si>
     <t xml:space="preserve">prespaccftaa</t>
@@ -5142,7 +5148,7 @@
       <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.91"/>
@@ -5752,7 +5758,7 @@
       <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.28"/>
@@ -5935,7 +5941,7 @@
       <selection pane="bottomRight" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.36"/>
@@ -8466,12 +8472,12 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+      <selection pane="bottomLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -10295,7 +10301,7 @@
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="26" t="s">
-        <v>247</v>
+        <v>185</v>
       </c>
       <c r="B88" s="26" t="str">
         <f aca="false">NODES!$A$29</f>
@@ -12345,17 +12351,17 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="26" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="B194" s="26" t="s">
         <v>109</v>
       </c>
       <c r="C194" s="42"/>
       <c r="D194" s="44" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="E194" s="42" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="F194" s="42"/>
       <c r="G194" s="42"/>
@@ -12372,24 +12378,24 @@
         <v>744</v>
       </c>
       <c r="E195" s="42" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="F195" s="42"/>
       <c r="G195" s="42"/>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="26" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="B196" s="26" t="s">
         <v>109</v>
       </c>
       <c r="C196" s="42"/>
       <c r="D196" s="44" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="E196" s="42" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="F196" s="42"/>
       <c r="G196" s="42"/>
@@ -12406,24 +12412,24 @@
         <v>744</v>
       </c>
       <c r="E197" s="42" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="F197" s="42"/>
       <c r="G197" s="42"/>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="26" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="B198" s="26" t="s">
         <v>109</v>
       </c>
       <c r="C198" s="42"/>
       <c r="D198" s="44" t="s">
-        <v>744</v>
+        <v>751</v>
       </c>
       <c r="E198" s="42" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="F198" s="42"/>
       <c r="G198" s="42"/>
@@ -12440,24 +12446,24 @@
         <v>744</v>
       </c>
       <c r="E199" s="42" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="F199" s="42"/>
       <c r="G199" s="42"/>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="26" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
       <c r="B200" s="26" t="s">
         <v>109</v>
       </c>
       <c r="C200" s="42"/>
       <c r="D200" s="44" t="s">
-        <v>744</v>
+        <v>751</v>
       </c>
       <c r="E200" s="42" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="F200" s="42"/>
       <c r="G200" s="42"/>
@@ -12474,7 +12480,7 @@
       <c r="C201" s="42"/>
       <c r="D201" s="42"/>
       <c r="E201" s="42" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="F201" s="42"/>
       <c r="G201" s="42"/>
@@ -12491,7 +12497,7 @@
       <c r="C202" s="42"/>
       <c r="D202" s="42"/>
       <c r="E202" s="42" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="F202" s="42"/>
       <c r="G202" s="42"/>
@@ -12508,7 +12514,7 @@
       <c r="C203" s="42"/>
       <c r="D203" s="42"/>
       <c r="E203" s="42" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="F203" s="42"/>
       <c r="G203" s="42"/>
@@ -12525,7 +12531,7 @@
       <c r="C204" s="42"/>
       <c r="D204" s="42"/>
       <c r="E204" s="42" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="F204" s="42"/>
       <c r="G204" s="42"/>
@@ -12542,7 +12548,7 @@
       <c r="C205" s="42"/>
       <c r="D205" s="42"/>
       <c r="E205" s="42" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="F205" s="42"/>
       <c r="G205" s="42"/>
@@ -12559,7 +12565,7 @@
       <c r="C206" s="42"/>
       <c r="D206" s="42"/>
       <c r="E206" s="42" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="F206" s="42"/>
       <c r="G206" s="42"/>
@@ -12576,7 +12582,7 @@
       <c r="C207" s="42"/>
       <c r="D207" s="42"/>
       <c r="E207" s="42" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="F207" s="42"/>
       <c r="G207" s="42"/>
@@ -12593,7 +12599,7 @@
       <c r="C208" s="42"/>
       <c r="D208" s="42"/>
       <c r="E208" s="42" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="F208" s="42"/>
       <c r="G208" s="42"/>
@@ -12610,7 +12616,7 @@
       <c r="C209" s="42"/>
       <c r="D209" s="42"/>
       <c r="E209" s="42" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="F209" s="42"/>
       <c r="G209" s="42"/>
@@ -12625,10 +12631,10 @@
       </c>
       <c r="C210" s="42"/>
       <c r="D210" s="42" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="E210" s="42" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="F210" s="42"/>
       <c r="G210" s="42"/>
@@ -12645,7 +12651,7 @@
       <c r="C211" s="42"/>
       <c r="D211" s="42"/>
       <c r="E211" s="42" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="F211" s="42"/>
       <c r="G211" s="42"/>
@@ -12660,10 +12666,10 @@
       </c>
       <c r="C212" s="42"/>
       <c r="D212" s="42" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="E212" s="42" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="F212" s="42"/>
       <c r="G212" s="42"/>
@@ -12678,10 +12684,10 @@
       </c>
       <c r="C213" s="42"/>
       <c r="D213" s="42" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="E213" s="42" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="F213" s="42"/>
       <c r="G213" s="42"/>
@@ -12696,10 +12702,10 @@
       </c>
       <c r="C214" s="42"/>
       <c r="D214" s="42" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="E214" s="42" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="F214" s="42"/>
       <c r="G214" s="42"/>
@@ -12714,10 +12720,10 @@
       </c>
       <c r="C215" s="42"/>
       <c r="D215" s="42" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="E215" s="42" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="F215" s="42"/>
       <c r="G215" s="42"/>
@@ -12732,10 +12738,10 @@
       </c>
       <c r="C216" s="42"/>
       <c r="D216" s="42" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="E216" s="42" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="F216" s="42"/>
       <c r="G216" s="42"/>
@@ -12749,10 +12755,10 @@
       </c>
       <c r="C217" s="42"/>
       <c r="D217" s="42" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="E217" s="42" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="F217" s="42"/>
       <c r="G217" s="42"/>
@@ -12769,7 +12775,7 @@
       <c r="C218" s="42"/>
       <c r="D218" s="42"/>
       <c r="E218" s="42" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="F218" s="42"/>
       <c r="G218" s="42"/>
@@ -12784,10 +12790,10 @@
       </c>
       <c r="C219" s="42"/>
       <c r="D219" s="42" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="E219" s="42" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="F219" s="42"/>
       <c r="G219" s="42"/>
@@ -12801,10 +12807,10 @@
       </c>
       <c r="C220" s="42"/>
       <c r="D220" s="44" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="E220" s="44" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="F220" s="42"/>
       <c r="G220" s="42"/>
@@ -12821,7 +12827,7 @@
       <c r="C221" s="42"/>
       <c r="D221" s="42"/>
       <c r="E221" s="42" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="F221" s="42"/>
       <c r="G221" s="42"/>
@@ -12836,10 +12842,10 @@
       </c>
       <c r="C222" s="42"/>
       <c r="D222" s="42" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="E222" s="42" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="F222" s="42"/>
       <c r="G222" s="42"/>
@@ -12853,10 +12859,10 @@
       </c>
       <c r="C223" s="42"/>
       <c r="D223" s="42" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="E223" s="44" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="F223" s="42"/>
       <c r="G223" s="42"/>
@@ -12872,10 +12878,10 @@
       </c>
       <c r="C224" s="42"/>
       <c r="D224" s="42" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="E224" s="42" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="F224" s="42"/>
       <c r="G224" s="42"/>
@@ -12892,7 +12898,7 @@
       <c r="C225" s="42"/>
       <c r="D225" s="42"/>
       <c r="E225" s="42" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="F225" s="42"/>
       <c r="G225" s="42"/>
@@ -12907,10 +12913,10 @@
       </c>
       <c r="C226" s="42"/>
       <c r="D226" s="42" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="E226" s="42" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="F226" s="42"/>
       <c r="G226" s="42"/>
@@ -12927,7 +12933,7 @@
       <c r="C227" s="42"/>
       <c r="D227" s="42"/>
       <c r="E227" s="42" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="F227" s="42"/>
       <c r="G227" s="42"/>
@@ -12942,10 +12948,10 @@
       </c>
       <c r="C228" s="42"/>
       <c r="D228" s="42" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="E228" s="42" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="F228" s="42"/>
       <c r="G228" s="42"/>
@@ -12959,10 +12965,10 @@
       </c>
       <c r="C229" s="42"/>
       <c r="D229" s="42" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="E229" s="42" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="F229" s="42"/>
       <c r="G229" s="42"/>
@@ -12979,7 +12985,7 @@
       <c r="C230" s="42"/>
       <c r="D230" s="42"/>
       <c r="E230" s="42" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="F230" s="42"/>
       <c r="G230" s="42"/>
@@ -12996,7 +13002,7 @@
       <c r="C231" s="42"/>
       <c r="D231" s="42"/>
       <c r="E231" s="42" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="F231" s="42"/>
       <c r="G231" s="42"/>
@@ -13012,10 +13018,10 @@
       </c>
       <c r="C232" s="42"/>
       <c r="D232" s="42" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="E232" s="42" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="F232" s="42"/>
       <c r="G232" s="42"/>
@@ -13030,10 +13036,10 @@
       </c>
       <c r="C233" s="42"/>
       <c r="D233" s="42" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="E233" s="42" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="F233" s="42"/>
       <c r="G233" s="42"/>
@@ -13050,7 +13056,7 @@
       <c r="C234" s="42"/>
       <c r="D234" s="42"/>
       <c r="E234" s="42" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="F234" s="42"/>
       <c r="G234" s="42"/>
@@ -13067,7 +13073,7 @@
       <c r="C235" s="42"/>
       <c r="D235" s="42"/>
       <c r="E235" s="42" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="F235" s="42"/>
       <c r="G235" s="42"/>
@@ -13084,7 +13090,7 @@
       <c r="C236" s="42"/>
       <c r="D236" s="42"/>
       <c r="E236" s="42" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="F236" s="42"/>
       <c r="G236" s="42"/>
@@ -13101,7 +13107,7 @@
       <c r="C237" s="42"/>
       <c r="D237" s="42"/>
       <c r="E237" s="42" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="F237" s="42"/>
       <c r="G237" s="42"/>
@@ -13118,7 +13124,7 @@
       <c r="C238" s="42"/>
       <c r="D238" s="42"/>
       <c r="E238" s="42" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="F238" s="42"/>
       <c r="G238" s="42"/>
@@ -13135,7 +13141,7 @@
       <c r="C239" s="42"/>
       <c r="D239" s="42"/>
       <c r="E239" s="42" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="F239" s="42"/>
       <c r="G239" s="42"/>
@@ -13152,7 +13158,7 @@
       <c r="C240" s="42"/>
       <c r="D240" s="42"/>
       <c r="E240" s="42" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="F240" s="42"/>
       <c r="G240" s="42"/>
@@ -13169,7 +13175,7 @@
       <c r="C241" s="42"/>
       <c r="D241" s="42"/>
       <c r="E241" s="42" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="F241" s="42"/>
       <c r="G241" s="42"/>
@@ -13186,7 +13192,7 @@
       <c r="C242" s="42"/>
       <c r="D242" s="42"/>
       <c r="E242" s="42" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="F242" s="42"/>
       <c r="G242" s="42"/>
@@ -13201,10 +13207,10 @@
       </c>
       <c r="C243" s="42"/>
       <c r="D243" s="42" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="E243" s="42" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="F243" s="42"/>
       <c r="G243" s="42"/>
@@ -13221,7 +13227,7 @@
       <c r="C244" s="42"/>
       <c r="D244" s="42"/>
       <c r="E244" s="42" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="F244" s="42"/>
       <c r="G244" s="42"/>
@@ -13237,10 +13243,10 @@
       </c>
       <c r="C245" s="42"/>
       <c r="D245" s="42" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="E245" s="42" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="F245" s="42"/>
       <c r="G245" s="42"/>
@@ -13254,10 +13260,10 @@
       </c>
       <c r="C246" s="42"/>
       <c r="D246" s="42" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="E246" s="42" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="F246" s="42"/>
       <c r="G246" s="42"/>
@@ -13274,7 +13280,7 @@
       <c r="C247" s="42"/>
       <c r="D247" s="42"/>
       <c r="E247" s="42" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="F247" s="42"/>
       <c r="G247" s="42"/>
@@ -13291,7 +13297,7 @@
       <c r="C248" s="42"/>
       <c r="D248" s="42"/>
       <c r="E248" s="42" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="F248" s="42"/>
       <c r="G248" s="42"/>
@@ -13305,10 +13311,10 @@
       </c>
       <c r="C249" s="42"/>
       <c r="D249" s="42" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="E249" s="42" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="F249" s="42"/>
       <c r="G249" s="42"/>
@@ -13322,10 +13328,10 @@
       </c>
       <c r="C250" s="42"/>
       <c r="D250" s="42" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="E250" s="42" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="F250" s="42"/>
       <c r="G250" s="42"/>
@@ -13339,10 +13345,10 @@
       </c>
       <c r="C251" s="42"/>
       <c r="D251" s="42" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="E251" s="42" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="F251" s="42"/>
       <c r="G251" s="42"/>
@@ -13356,10 +13362,10 @@
       </c>
       <c r="C252" s="42"/>
       <c r="D252" s="44" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="E252" s="44" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="F252" s="42"/>
       <c r="G252" s="42"/>
@@ -13373,10 +13379,10 @@
       </c>
       <c r="C253" s="42"/>
       <c r="D253" s="44" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="E253" s="44" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="F253" s="42"/>
       <c r="G253" s="42"/>
@@ -13390,10 +13396,10 @@
       </c>
       <c r="C254" s="42"/>
       <c r="D254" s="44" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="E254" s="44" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="F254" s="42"/>
       <c r="G254" s="42"/>
@@ -13407,10 +13413,10 @@
       </c>
       <c r="C255" s="42"/>
       <c r="D255" s="44" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="E255" s="44" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="F255" s="42"/>
       <c r="G255" s="42"/>
@@ -13424,10 +13430,10 @@
       </c>
       <c r="C256" s="42"/>
       <c r="D256" s="44" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="E256" s="44" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="F256" s="42"/>
       <c r="G256" s="42"/>
@@ -13441,10 +13447,10 @@
       </c>
       <c r="C257" s="42"/>
       <c r="D257" s="44" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="E257" s="44" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="F257" s="42"/>
       <c r="G257" s="42"/>
@@ -13458,10 +13464,10 @@
       </c>
       <c r="C258" s="42"/>
       <c r="D258" s="44" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="E258" s="44" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="F258" s="42"/>
       <c r="G258" s="42"/>
@@ -13475,10 +13481,10 @@
       </c>
       <c r="C259" s="42"/>
       <c r="D259" s="44" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="E259" s="44" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="F259" s="42"/>
       <c r="G259" s="42"/>
@@ -13492,10 +13498,10 @@
       </c>
       <c r="C260" s="42"/>
       <c r="D260" s="44" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="E260" s="44" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="F260" s="42"/>
       <c r="G260" s="42"/>
@@ -13509,10 +13515,10 @@
       </c>
       <c r="C261" s="42"/>
       <c r="D261" s="44" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="E261" s="44" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="F261" s="42"/>
       <c r="G261" s="42"/>
@@ -13526,10 +13532,10 @@
       </c>
       <c r="C262" s="42"/>
       <c r="D262" s="44" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="E262" s="44" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="F262" s="42"/>
       <c r="G262" s="42"/>
@@ -13543,10 +13549,10 @@
       </c>
       <c r="C263" s="42"/>
       <c r="D263" s="44" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="E263" s="44" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="F263" s="42"/>
       <c r="G263" s="42"/>
@@ -13560,10 +13566,10 @@
       </c>
       <c r="C264" s="42"/>
       <c r="D264" s="44" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="E264" s="44" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="F264" s="42"/>
       <c r="G264" s="42"/>
@@ -13577,10 +13583,10 @@
       </c>
       <c r="C265" s="42"/>
       <c r="D265" s="44" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="E265" s="44" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="F265" s="42"/>
       <c r="G265" s="42"/>
@@ -13594,10 +13600,10 @@
       </c>
       <c r="C266" s="42"/>
       <c r="D266" s="44" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="E266" s="44" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="F266" s="42"/>
       <c r="G266" s="42"/>
@@ -13611,10 +13617,10 @@
       </c>
       <c r="C267" s="42"/>
       <c r="D267" s="44" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="E267" s="44" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="F267" s="42"/>
       <c r="G267" s="42"/>
@@ -13628,10 +13634,10 @@
       </c>
       <c r="C268" s="42"/>
       <c r="D268" s="44" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="E268" s="44" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="F268" s="42"/>
       <c r="G268" s="42"/>
@@ -13645,10 +13651,10 @@
       </c>
       <c r="C269" s="42"/>
       <c r="D269" s="44" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="E269" s="44" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
       <c r="F269" s="42"/>
       <c r="G269" s="42"/>
@@ -13662,10 +13668,10 @@
       </c>
       <c r="C270" s="42"/>
       <c r="D270" s="44" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="E270" s="44" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="F270" s="42"/>
       <c r="G270" s="42"/>
@@ -13679,10 +13685,10 @@
       </c>
       <c r="C271" s="42"/>
       <c r="D271" s="44" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
       <c r="E271" s="44" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="F271" s="42"/>
       <c r="G271" s="42"/>
@@ -13696,10 +13702,10 @@
       </c>
       <c r="C272" s="42"/>
       <c r="D272" s="44" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="E272" s="44" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
       <c r="F272" s="42"/>
       <c r="G272" s="42"/>
@@ -13713,10 +13719,10 @@
       </c>
       <c r="C273" s="42"/>
       <c r="D273" s="44" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="E273" s="44" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="F273" s="42"/>
       <c r="G273" s="42"/>
@@ -13730,10 +13736,10 @@
       </c>
       <c r="C274" s="42"/>
       <c r="D274" s="44" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="E274" s="44" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="F274" s="42"/>
       <c r="G274" s="42"/>
@@ -13747,10 +13753,10 @@
       </c>
       <c r="C275" s="42"/>
       <c r="D275" s="44" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="E275" s="44" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="F275" s="42"/>
       <c r="G275" s="42"/>
@@ -13764,10 +13770,10 @@
       </c>
       <c r="C276" s="42"/>
       <c r="D276" s="44" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="E276" s="44" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="F276" s="42"/>
       <c r="G276" s="42"/>
@@ -13781,10 +13787,10 @@
       </c>
       <c r="C277" s="42"/>
       <c r="D277" s="44" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="E277" s="44" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="F277" s="42"/>
       <c r="G277" s="42"/>
@@ -13798,10 +13804,10 @@
       </c>
       <c r="C278" s="42"/>
       <c r="D278" s="44" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="E278" s="44" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="F278" s="42"/>
       <c r="G278" s="42"/>
@@ -13815,10 +13821,10 @@
       </c>
       <c r="C279" s="42"/>
       <c r="D279" s="44" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="E279" s="44" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="F279" s="42"/>
       <c r="G279" s="42"/>
@@ -13833,7 +13839,7 @@
       <c r="C280" s="42"/>
       <c r="D280" s="44"/>
       <c r="E280" s="44" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="F280" s="42"/>
       <c r="G280" s="42"/>
@@ -13848,7 +13854,7 @@
       <c r="C281" s="42"/>
       <c r="D281" s="44"/>
       <c r="E281" s="44" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="F281" s="42"/>
       <c r="G281" s="42"/>
@@ -13863,7 +13869,7 @@
       <c r="C282" s="42"/>
       <c r="D282" s="44"/>
       <c r="E282" s="44" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="F282" s="42"/>
       <c r="G282" s="42"/>
@@ -13878,7 +13884,7 @@
       <c r="C283" s="42"/>
       <c r="D283" s="44"/>
       <c r="E283" s="44" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="F283" s="42"/>
       <c r="G283" s="42"/>
@@ -13893,7 +13899,7 @@
       <c r="C284" s="42"/>
       <c r="D284" s="44"/>
       <c r="E284" s="44" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="F284" s="42"/>
       <c r="G284" s="42"/>
@@ -13908,7 +13914,7 @@
       <c r="C285" s="42"/>
       <c r="D285" s="44"/>
       <c r="E285" s="44" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="F285" s="42"/>
       <c r="G285" s="42"/>
@@ -13923,7 +13929,7 @@
       <c r="C286" s="42"/>
       <c r="D286" s="44"/>
       <c r="E286" s="44" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="F286" s="42"/>
       <c r="G286" s="42"/>
@@ -13938,7 +13944,7 @@
       <c r="C287" s="42"/>
       <c r="D287" s="44"/>
       <c r="E287" s="44" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="F287" s="42"/>
       <c r="G287" s="42"/>
@@ -13953,7 +13959,7 @@
       <c r="C288" s="42"/>
       <c r="D288" s="44"/>
       <c r="E288" s="44" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="F288" s="42"/>
       <c r="G288" s="42"/>
@@ -13968,7 +13974,7 @@
       <c r="C289" s="42"/>
       <c r="D289" s="44"/>
       <c r="E289" s="44" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="F289" s="42"/>
       <c r="G289" s="42"/>
@@ -13983,7 +13989,7 @@
       <c r="C290" s="42"/>
       <c r="D290" s="44"/>
       <c r="E290" s="44" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="F290" s="42"/>
       <c r="G290" s="42"/>
@@ -13998,7 +14004,7 @@
       <c r="C291" s="42"/>
       <c r="D291" s="44"/>
       <c r="E291" s="44" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="F291" s="42"/>
       <c r="G291" s="42"/>
@@ -14013,7 +14019,7 @@
       <c r="C292" s="42"/>
       <c r="D292" s="44"/>
       <c r="E292" s="44" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="F292" s="42"/>
       <c r="G292" s="42"/>
@@ -14028,7 +14034,7 @@
       <c r="C293" s="42"/>
       <c r="D293" s="44"/>
       <c r="E293" s="44" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="F293" s="42"/>
       <c r="G293" s="42"/>
@@ -14042,10 +14048,10 @@
       </c>
       <c r="C294" s="42"/>
       <c r="D294" s="44" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="E294" s="44" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="F294" s="42"/>
       <c r="G294" s="42"/>
@@ -14059,10 +14065,10 @@
       </c>
       <c r="C295" s="42"/>
       <c r="D295" s="44" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="E295" s="44" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="F295" s="42"/>
       <c r="G295" s="42"/>
@@ -14076,10 +14082,10 @@
       </c>
       <c r="C296" s="42"/>
       <c r="D296" s="44" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="E296" s="44" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="F296" s="42"/>
       <c r="G296" s="42"/>
@@ -14094,7 +14100,7 @@
       <c r="C297" s="42"/>
       <c r="D297" s="44"/>
       <c r="E297" s="44" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="F297" s="42"/>
       <c r="G297" s="42"/>
@@ -14109,7 +14115,7 @@
       <c r="C298" s="42"/>
       <c r="D298" s="44"/>
       <c r="E298" s="44" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="F298" s="42"/>
       <c r="G298" s="42"/>
@@ -14123,10 +14129,10 @@
       </c>
       <c r="C299" s="42"/>
       <c r="D299" s="44" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="E299" s="44" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="F299" s="42"/>
       <c r="G299" s="42"/>
@@ -14140,10 +14146,10 @@
       </c>
       <c r="C300" s="42"/>
       <c r="D300" s="44" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="E300" s="44" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="F300" s="42"/>
       <c r="G300" s="42"/>
@@ -14157,10 +14163,10 @@
       </c>
       <c r="C301" s="42"/>
       <c r="D301" s="44" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="E301" s="44" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="F301" s="42"/>
       <c r="G301" s="42"/>
@@ -14174,10 +14180,10 @@
       </c>
       <c r="C302" s="42"/>
       <c r="D302" s="44" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="E302" s="44" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="F302" s="42"/>
       <c r="G302" s="42"/>
@@ -14191,10 +14197,10 @@
       </c>
       <c r="C303" s="42"/>
       <c r="D303" s="44" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="E303" s="44" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="F303" s="42"/>
       <c r="G303" s="42"/>
@@ -14208,10 +14214,10 @@
       </c>
       <c r="C304" s="42"/>
       <c r="D304" s="44" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="E304" s="44" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="F304" s="42"/>
       <c r="G304" s="42"/>
@@ -14245,7 +14251,7 @@
       <selection pane="bottomLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -14288,10 +14294,10 @@
       </c>
       <c r="C2" s="42"/>
       <c r="D2" s="42" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
@@ -14305,10 +14311,10 @@
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="44" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -14322,10 +14328,10 @@
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="44" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
@@ -14339,10 +14345,10 @@
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="44" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
@@ -14356,10 +14362,10 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="44" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42"/>
@@ -14373,10 +14379,10 @@
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="44" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
@@ -14390,10 +14396,10 @@
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="44" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="F8" s="42"/>
       <c r="G8" s="42"/>
@@ -14407,10 +14413,10 @@
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="44" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
@@ -14424,10 +14430,10 @@
       </c>
       <c r="C10" s="42"/>
       <c r="D10" s="44" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
@@ -14441,10 +14447,10 @@
       </c>
       <c r="C11" s="42"/>
       <c r="D11" s="44" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
@@ -14458,10 +14464,10 @@
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="44" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
@@ -14475,10 +14481,10 @@
       </c>
       <c r="C13" s="42"/>
       <c r="D13" s="44" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
@@ -14492,10 +14498,10 @@
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="44" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="E14" s="44" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="F14" s="42"/>
       <c r="G14" s="42"/>
@@ -14509,10 +14515,10 @@
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="44" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="F15" s="42"/>
       <c r="G15" s="42"/>
@@ -14526,10 +14532,10 @@
       </c>
       <c r="C16" s="42"/>
       <c r="D16" s="44" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="E16" s="44" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
@@ -14543,10 +14549,10 @@
       </c>
       <c r="C17" s="42"/>
       <c r="D17" s="44" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="F17" s="42"/>
       <c r="G17" s="42"/>
@@ -14560,10 +14566,10 @@
       </c>
       <c r="C18" s="42"/>
       <c r="D18" s="44" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="F18" s="42"/>
       <c r="G18" s="42"/>
@@ -14577,10 +14583,10 @@
       </c>
       <c r="C19" s="42"/>
       <c r="D19" s="44" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="F19" s="42"/>
       <c r="G19" s="42"/>
@@ -14594,10 +14600,10 @@
       </c>
       <c r="C20" s="42"/>
       <c r="D20" s="44" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="F20" s="42"/>
       <c r="G20" s="42"/>
@@ -14611,10 +14617,10 @@
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="44" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="F21" s="42"/>
       <c r="G21" s="42"/>
@@ -14628,10 +14634,10 @@
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="44" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="F22" s="42"/>
       <c r="G22" s="42"/>
@@ -14645,10 +14651,10 @@
       </c>
       <c r="C23" s="42"/>
       <c r="D23" s="44" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="E23" s="44" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="F23" s="42"/>
       <c r="G23" s="42"/>
@@ -14662,10 +14668,10 @@
       </c>
       <c r="C24" s="42"/>
       <c r="D24" s="44" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="F24" s="42"/>
       <c r="G24" s="42"/>
@@ -14679,10 +14685,10 @@
       </c>
       <c r="C25" s="42"/>
       <c r="D25" s="44" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="E25" s="44" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="F25" s="42"/>
       <c r="G25" s="42"/>
@@ -14696,10 +14702,10 @@
       </c>
       <c r="C26" s="42"/>
       <c r="D26" s="44" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
       <c r="F26" s="42"/>
       <c r="G26" s="42"/>
@@ -14713,10 +14719,10 @@
       </c>
       <c r="C27" s="42"/>
       <c r="D27" s="44" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="F27" s="42"/>
       <c r="G27" s="42"/>
@@ -14730,10 +14736,10 @@
       </c>
       <c r="C28" s="42"/>
       <c r="D28" s="44" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E28" s="44" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
       <c r="F28" s="42"/>
       <c r="G28" s="42"/>
@@ -14747,10 +14753,10 @@
       </c>
       <c r="C29" s="42"/>
       <c r="D29" s="44" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="E29" s="44" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="F29" s="42"/>
       <c r="G29" s="42"/>
@@ -14764,10 +14770,10 @@
       </c>
       <c r="C30" s="42"/>
       <c r="D30" s="44" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E30" s="44" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
       <c r="F30" s="42"/>
       <c r="G30" s="42"/>
@@ -14781,10 +14787,10 @@
       </c>
       <c r="C31" s="42"/>
       <c r="D31" s="44" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="E31" s="44" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="F31" s="42"/>
       <c r="G31" s="42"/>
@@ -14797,13 +14803,13 @@
         <v>327</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="D32" s="44" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="E32" s="44" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="F32" s="42"/>
       <c r="G32" s="42"/>
@@ -14819,10 +14825,10 @@
         <v>125</v>
       </c>
       <c r="D33" s="44" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E33" s="44" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="F33" s="42"/>
       <c r="G33" s="42"/>
@@ -14838,10 +14844,10 @@
         <v>132</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="E34" s="44" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="F34" s="42"/>
       <c r="G34" s="42"/>
@@ -14857,10 +14863,10 @@
         <v>118</v>
       </c>
       <c r="D35" s="44" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="E35" s="44" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="F35" s="42"/>
       <c r="G35" s="42"/>
@@ -14873,13 +14879,13 @@
         <v>327</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="D36" s="44" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="E36" s="44" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="F36" s="42"/>
       <c r="G36" s="42"/>
@@ -14893,10 +14899,10 @@
       </c>
       <c r="C37" s="42"/>
       <c r="D37" s="44" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="E37" s="44" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="F37" s="42"/>
       <c r="G37" s="42"/>
@@ -14913,7 +14919,7 @@
         <v>344</v>
       </c>
       <c r="E38" s="44" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="F38" s="42"/>
       <c r="G38" s="42"/>
@@ -14927,10 +14933,10 @@
       </c>
       <c r="C39" s="42"/>
       <c r="D39" s="44" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="E39" s="44" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
       <c r="F39" s="42"/>
       <c r="G39" s="42"/>
@@ -14944,10 +14950,10 @@
       </c>
       <c r="C40" s="42"/>
       <c r="D40" s="44" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="E40" s="44" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="F40" s="42"/>
       <c r="G40" s="42"/>
@@ -14960,13 +14966,13 @@
         <v>349</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="D41" s="44" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
       <c r="E41" s="44" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="F41" s="42"/>
       <c r="G41" s="42"/>
@@ -14980,10 +14986,10 @@
       </c>
       <c r="C42" s="42"/>
       <c r="D42" s="44" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E42" s="44" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
       <c r="F42" s="42"/>
       <c r="G42" s="42"/>
@@ -14997,10 +15003,10 @@
       </c>
       <c r="C43" s="42"/>
       <c r="D43" s="44" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E43" s="44" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="F43" s="42"/>
       <c r="G43" s="42"/>
@@ -15014,10 +15020,10 @@
       </c>
       <c r="C44" s="42"/>
       <c r="D44" s="44" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E44" s="44" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="F44" s="42"/>
       <c r="G44" s="42"/>
@@ -15031,10 +15037,10 @@
       </c>
       <c r="C45" s="42"/>
       <c r="D45" s="44" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E45" s="44" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="F45" s="42"/>
       <c r="G45" s="42"/>
@@ -15048,10 +15054,10 @@
       </c>
       <c r="C46" s="42"/>
       <c r="D46" s="44" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="E46" s="44" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
       <c r="F46" s="42"/>
       <c r="G46" s="42"/>
@@ -15065,10 +15071,10 @@
       </c>
       <c r="C47" s="42"/>
       <c r="D47" s="44" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="E47" s="44" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="F47" s="42"/>
       <c r="G47" s="42"/>
@@ -15082,10 +15088,10 @@
       </c>
       <c r="C48" s="42"/>
       <c r="D48" s="44" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="E48" s="44" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="F48" s="42"/>
       <c r="G48" s="42"/>
@@ -15099,10 +15105,10 @@
       </c>
       <c r="C49" s="42"/>
       <c r="D49" s="44" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="E49" s="44" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="F49" s="42"/>
       <c r="G49" s="42"/>
@@ -15116,10 +15122,10 @@
       </c>
       <c r="C50" s="42"/>
       <c r="D50" s="44" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E50" s="50" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="F50" s="42"/>
       <c r="G50" s="42"/>
@@ -15133,10 +15139,10 @@
       </c>
       <c r="C51" s="42"/>
       <c r="D51" s="44" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E51" s="50" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="F51" s="42"/>
       <c r="G51" s="42"/>
@@ -15153,7 +15159,7 @@
         <v>354</v>
       </c>
       <c r="E52" s="50" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="F52" s="42"/>
       <c r="G52" s="42"/>
@@ -15170,7 +15176,7 @@
         <v>354</v>
       </c>
       <c r="E53" s="50" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="F53" s="42"/>
       <c r="G53" s="42"/>
@@ -15184,10 +15190,10 @@
       </c>
       <c r="C54" s="42"/>
       <c r="D54" s="44" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="E54" s="50" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="F54" s="42"/>
       <c r="G54" s="42"/>
@@ -15204,7 +15210,7 @@
         <v>498</v>
       </c>
       <c r="E55" s="50" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="F55" s="42"/>
       <c r="G55" s="42"/>
@@ -15217,13 +15223,13 @@
         <v>327</v>
       </c>
       <c r="C56" s="42" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="D56" s="44" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="E56" s="50" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="F56" s="42"/>
       <c r="G56" s="42"/>
@@ -15237,10 +15243,10 @@
       </c>
       <c r="C57" s="42"/>
       <c r="D57" s="44" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="E57" s="50" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="F57" s="42"/>
       <c r="G57" s="42"/>
@@ -15254,10 +15260,10 @@
       </c>
       <c r="C58" s="42"/>
       <c r="D58" s="44" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="E58" s="50" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="F58" s="42"/>
       <c r="G58" s="42"/>
@@ -15274,7 +15280,7 @@
         <v>146</v>
       </c>
       <c r="E59" s="50" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="F59" s="42"/>
       <c r="G59" s="42"/>
@@ -15291,7 +15297,7 @@
         <v>361</v>
       </c>
       <c r="E60" s="50" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="F60" s="42"/>
       <c r="G60" s="42"/>
@@ -15305,10 +15311,10 @@
       </c>
       <c r="C61" s="42"/>
       <c r="D61" s="44" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="E61" s="44" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="F61" s="42"/>
       <c r="G61" s="42"/>
@@ -15322,10 +15328,10 @@
       </c>
       <c r="C62" s="42"/>
       <c r="D62" s="44" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E62" s="44" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="F62" s="42"/>
       <c r="G62" s="42"/>
@@ -15339,10 +15345,10 @@
       </c>
       <c r="C63" s="42"/>
       <c r="D63" s="44" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E63" s="44" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="F63" s="42"/>
       <c r="G63" s="42"/>
@@ -15356,10 +15362,10 @@
       </c>
       <c r="C64" s="42"/>
       <c r="D64" s="44" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E64" s="44" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="F64" s="42"/>
       <c r="G64" s="42"/>
@@ -15373,10 +15379,10 @@
       </c>
       <c r="C65" s="42"/>
       <c r="D65" s="44" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
       <c r="E65" s="44" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="F65" s="42"/>
       <c r="G65" s="42"/>
@@ -15390,10 +15396,10 @@
       </c>
       <c r="C66" s="42"/>
       <c r="D66" s="44" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="E66" s="44" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="F66" s="42"/>
       <c r="G66" s="42"/>
@@ -15407,10 +15413,10 @@
       </c>
       <c r="C67" s="42"/>
       <c r="D67" s="44" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="E67" s="44" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="F67" s="42"/>
       <c r="G67" s="42"/>
@@ -15424,10 +15430,10 @@
       </c>
       <c r="C68" s="42"/>
       <c r="D68" s="44" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="E68" s="44" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="F68" s="42"/>
       <c r="G68" s="42"/>
@@ -15670,7 +15676,7 @@
       <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -15713,10 +15719,10 @@
       </c>
       <c r="C2" s="42"/>
       <c r="D2" s="42" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="F2" s="42"/>
       <c r="G2" s="42"/>
@@ -15730,10 +15736,10 @@
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="44" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="F3" s="42"/>
       <c r="G3" s="42"/>
@@ -15747,10 +15753,10 @@
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="44" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="F4" s="42"/>
       <c r="G4" s="42"/>
@@ -15764,10 +15770,10 @@
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="44" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="F5" s="42"/>
       <c r="G5" s="42"/>
@@ -15781,112 +15787,112 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="44" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="F6" s="42"/>
       <c r="G6" s="42"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="48" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>222</v>
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="44" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="F7" s="42"/>
       <c r="G7" s="42"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="48" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>222</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="44" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="F8" s="42"/>
       <c r="G8" s="42"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="48" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B9" s="26" t="s">
         <v>222</v>
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="44" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="F9" s="42"/>
       <c r="G9" s="42"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="48" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>222</v>
       </c>
       <c r="C10" s="42"/>
       <c r="D10" s="44" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>222</v>
       </c>
       <c r="C11" s="42"/>
       <c r="D11" s="44" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="F11" s="42"/>
       <c r="G11" s="42"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="48" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>222</v>
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="44" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="F12" s="42"/>
       <c r="G12" s="42"/>
@@ -15900,218 +15906,218 @@
       </c>
       <c r="C13" s="42"/>
       <c r="D13" s="44" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="F13" s="42"/>
       <c r="G13" s="42"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="48" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B14" s="26" t="s">
         <v>220</v>
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="44" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="E14" s="44" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="F14" s="42"/>
       <c r="G14" s="42"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="48" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B15" s="26" t="s">
         <v>220</v>
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="44" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="F15" s="42"/>
       <c r="G15" s="42"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="48" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>220</v>
       </c>
       <c r="C16" s="42"/>
       <c r="D16" s="44" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E16" s="44" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="48" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B17" s="26" t="s">
         <v>220</v>
       </c>
       <c r="C17" s="42"/>
       <c r="D17" s="44" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="F17" s="42"/>
       <c r="G17" s="42"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="48" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>222</v>
       </c>
       <c r="C18" s="42"/>
       <c r="D18" s="44" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
       <c r="F18" s="42"/>
       <c r="G18" s="42"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="48" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B19" s="26" t="s">
         <v>220</v>
       </c>
       <c r="C19" s="42" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="D19" s="44" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="F19" s="42"/>
       <c r="G19" s="42"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="48" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>220</v>
       </c>
       <c r="C20" s="42"/>
       <c r="D20" s="44" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="E20" s="44" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
       <c r="F20" s="42"/>
       <c r="G20" s="42"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="48" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>220</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="44" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="E21" s="44" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="F21" s="42"/>
       <c r="G21" s="42"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="48" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>220</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="44" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
       <c r="E22" s="44" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="F22" s="42"/>
       <c r="G22" s="42"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="48" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>220</v>
       </c>
       <c r="C23" s="42"/>
       <c r="D23" s="44" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
       <c r="E23" s="44" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="F23" s="42"/>
       <c r="G23" s="42"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="48" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>232</v>
       </c>
       <c r="C24" s="42"/>
       <c r="D24" s="44" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
       <c r="F24" s="42"/>
       <c r="G24" s="42"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="48" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="B25" s="26" t="s">
         <v>232</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="D25" s="44" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="E25" s="50" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
       <c r="F25" s="42"/>
       <c r="G25" s="42"/>
@@ -16128,24 +16134,24 @@
         <v>344</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="F26" s="42"/>
       <c r="G26" s="42"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="48" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="B27" s="26" t="s">
         <v>222</v>
       </c>
       <c r="C27" s="42"/>
       <c r="D27" s="44" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="F27" s="42"/>
       <c r="G27" s="42"/>
@@ -16159,10 +16165,10 @@
       </c>
       <c r="C28" s="42"/>
       <c r="D28" s="44" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="E28" s="44" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="F28" s="42"/>
       <c r="G28" s="42"/>
@@ -16176,10 +16182,10 @@
       </c>
       <c r="C29" s="42"/>
       <c r="D29" s="44" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="E29" s="43" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
       <c r="F29" s="42"/>
       <c r="G29" s="42"/>
@@ -16196,7 +16202,7 @@
         <v>354</v>
       </c>
       <c r="E30" s="50" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="F30" s="42"/>
       <c r="G30" s="42"/>
@@ -16213,7 +16219,7 @@
         <v>361</v>
       </c>
       <c r="E31" s="50" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="F31" s="42"/>
       <c r="G31" s="42"/>
@@ -16230,7 +16236,7 @@
         <v>146</v>
       </c>
       <c r="E32" s="50" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
       <c r="F32" s="42"/>
       <c r="G32" s="42"/>
@@ -16244,10 +16250,10 @@
       </c>
       <c r="C33" s="42"/>
       <c r="D33" s="49" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
       <c r="E33" s="44" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="F33" s="42"/>
       <c r="G33" s="42"/>
@@ -16261,10 +16267,10 @@
       </c>
       <c r="C34" s="42"/>
       <c r="D34" s="44" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E34" s="50" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="F34" s="42"/>
       <c r="G34" s="42"/>
@@ -16296,7 +16302,7 @@
       <selection pane="bottomLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -16323,563 +16329,563 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C2" s="53" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D2" s="54" t="s">
         <v>1027</v>
       </c>
-      <c r="D2" s="54" t="s">
-        <v>1025</v>
-      </c>
       <c r="E2" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="B3" s="52" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E3" s="55" t="s">
         <v>1030</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>1031</v>
-      </c>
-      <c r="D3" s="54" t="s">
-        <v>1029</v>
-      </c>
-      <c r="E3" s="55" t="s">
-        <v>1028</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="D4" s="54" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
       <c r="C7" s="56" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="E7" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="C10" s="53" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="C11" s="53" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="E11" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="C12" s="53" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="E12" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="C13" s="56" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="B14" s="52" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C14" s="56" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E14" s="57" t="s">
         <v>1054</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>1031</v>
-      </c>
-      <c r="D14" s="54" t="s">
-        <v>1053</v>
-      </c>
-      <c r="E14" s="57" t="s">
-        <v>1052</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="C15" s="56" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D15" s="54" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="C16" s="56" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="C17" s="56" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="E17" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
       <c r="C19" s="56" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D19" s="54" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="C20" s="53" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="D20" s="54" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="E20" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="B21" s="59" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="C21" s="53" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D21" s="54" t="s">
         <v>1071</v>
       </c>
-      <c r="D21" s="54" t="s">
-        <v>1069</v>
-      </c>
       <c r="E21" s="55" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B22" s="60" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C22" s="53" t="s">
         <v>1073</v>
       </c>
-      <c r="B22" s="60" t="s">
-        <v>1074</v>
-      </c>
-      <c r="C22" s="53" t="s">
-        <v>1071</v>
-      </c>
       <c r="D22" s="54" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="E22" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
       <c r="C23" s="53" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="D23" s="54" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="E23" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="B24" s="52" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="C24" s="53" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="D24" s="54" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="E24" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="B25" s="52" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="C25" s="53" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D25" s="54" t="s">
         <v>1082</v>
       </c>
-      <c r="D25" s="54" t="s">
-        <v>1080</v>
-      </c>
       <c r="E25" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="C26" s="53" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="D26" s="62" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="E26" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="D27" s="62" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="E27" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="B28" s="61" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="D28" s="62" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="E28" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="B29" s="61" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="C29" s="63" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="D29" s="62" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="E29" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
       <c r="B30" s="61" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="C30" s="53" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="D30" s="62" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="E30" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="B31" s="61" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="D31" s="62" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
       <c r="E31" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="C32" s="53" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
       <c r="D32" s="54" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="E32" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="C33" s="56" t="s">
+        <v>1107</v>
+      </c>
+      <c r="D33" s="62" t="s">
         <v>1105</v>
       </c>
-      <c r="D33" s="62" t="s">
-        <v>1103</v>
-      </c>
       <c r="E33" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="B34" s="58" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C34" s="56" t="s">
         <v>1107</v>
       </c>
-      <c r="C34" s="56" t="s">
-        <v>1105</v>
-      </c>
       <c r="D34" s="54" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="E34" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
   </sheetData>
@@ -16913,7 +16919,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -16940,274 +16946,274 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="C2" s="53"/>
       <c r="D2" s="54" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="E2" s="64" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
       <c r="B3" s="52" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="C3" s="53" t="s">
+        <v>1114</v>
+      </c>
+      <c r="D3" s="54" t="s">
         <v>1112</v>
       </c>
-      <c r="D3" s="54" t="s">
-        <v>1110</v>
-      </c>
       <c r="E3" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="C4" s="53"/>
       <c r="D4" s="54" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="E4" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="C5" s="53"/>
       <c r="D5" s="54" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
       <c r="E5" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="C6" s="53"/>
       <c r="D6" s="54" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="E6" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="C7" s="53"/>
       <c r="D7" s="54" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="E7" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="C8" s="53"/>
       <c r="D8" s="54" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="E8" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="B9" s="52" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="C9" s="53"/>
       <c r="D9" s="54" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
       <c r="E9" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="B10" s="52" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="C10" s="53"/>
       <c r="D10" s="54" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="E10" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="C11" s="53"/>
       <c r="D11" s="54" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="E11" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="B12" s="52" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="C12" s="53"/>
       <c r="D12" s="54" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
       <c r="E12" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="B13" s="52" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
       <c r="C13" s="53"/>
       <c r="D13" s="54" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="E13" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="B14" s="52" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="C14" s="53"/>
       <c r="D14" s="54" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="B15" s="52" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="C15" s="53"/>
       <c r="D15" s="54" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="B16" s="52" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="C16" s="53"/>
       <c r="D16" s="54" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="B17" s="52" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
       <c r="C17" s="53"/>
       <c r="D17" s="54" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="E17" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="C18" s="53"/>
       <c r="D18" s="54" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="E18" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="B19" s="52" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="C19" s="53"/>
       <c r="D19" s="54" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
       <c r="E19" s="57" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
     </row>
   </sheetData>
@@ -17238,7 +17244,7 @@
       <selection pane="bottomRight" activeCell="AQ9" activeCellId="0" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2734375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.27"/>

</xml_diff>

<commit_message>
improve CO2 plots in sepia
</commit_message>
<xml_diff>
--- a/SEPIA/SEPIA_config.xlsx
+++ b/SEPIA/SEPIA_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" state="visible" r:id="rId2"/>
@@ -5148,7 +5148,7 @@
       <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.91"/>
@@ -5758,7 +5758,7 @@
       <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.28"/>
@@ -5941,7 +5941,7 @@
       <selection pane="bottomRight" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.36"/>
@@ -8471,13 +8471,13 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A88" activeCellId="0" sqref="A88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -14251,7 +14251,7 @@
       <selection pane="bottomLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -15670,13 +15670,13 @@
   </sheetPr>
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="bottomLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -16195,7 +16195,7 @@
         <v>353</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>239</v>
+        <v>353</v>
       </c>
       <c r="C30" s="42"/>
       <c r="D30" s="44" t="s">
@@ -16263,7 +16263,7 @@
         <v>355</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>224</v>
+        <v>355</v>
       </c>
       <c r="C34" s="42"/>
       <c r="D34" s="44" t="s">
@@ -16302,7 +16302,7 @@
       <selection pane="bottomLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -16919,7 +16919,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -17244,7 +17244,7 @@
       <selection pane="bottomRight" activeCell="AQ9" activeCellId="0" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="11.30859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.27"/>

</xml_diff>

<commit_message>
adding combined country graphs in scenario results
</commit_message>
<xml_diff>
--- a/SEPIA/SEPIA_config.xlsx
+++ b/SEPIA/SEPIA_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" state="visible" r:id="rId2"/>
@@ -447,7 +447,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2169" uniqueCount="1141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2165" uniqueCount="1140">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -3363,9 +3363,6 @@
   </si>
   <si>
     <t xml:space="preserve">emmgasccx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emmgasccxx</t>
   </si>
   <si>
     <t xml:space="preserve">solid biomass for industry CC</t>
@@ -8476,8 +8473,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E108" activeCellId="0" sqref="E108"/>
     </sheetView>
@@ -14064,10 +14061,10 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E69" activeCellId="0" sqref="E69"/>
+      <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14832,65 +14829,65 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="51" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>328</v>
+        <v>352</v>
       </c>
       <c r="C44" s="44"/>
       <c r="D44" s="46" t="s">
-        <v>969</v>
+        <v>972</v>
       </c>
       <c r="E44" s="46" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="F44" s="44"/>
       <c r="G44" s="44"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="51" t="s">
-        <v>328</v>
+        <v>352</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
       <c r="C45" s="44"/>
       <c r="D45" s="46" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="E45" s="46" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="F45" s="44"/>
       <c r="G45" s="44"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="51" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C46" s="44"/>
       <c r="D46" s="46" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="E46" s="46" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="F46" s="44"/>
       <c r="G46" s="44"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="51" t="s">
+        <v>328</v>
+      </c>
+      <c r="B47" s="28" t="s">
         <v>340</v>
-      </c>
-      <c r="B47" s="28" t="s">
-        <v>328</v>
       </c>
       <c r="C47" s="44"/>
       <c r="D47" s="46" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="E47" s="46" t="s">
         <v>978</v>
@@ -14900,48 +14897,48 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="51" t="s">
+        <v>336</v>
+      </c>
+      <c r="B48" s="28" t="s">
         <v>328</v>
-      </c>
-      <c r="B48" s="28" t="s">
-        <v>340</v>
       </c>
       <c r="C48" s="44"/>
       <c r="D48" s="46" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="E48" s="46" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="F48" s="44"/>
       <c r="G48" s="44"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="51" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="C49" s="44"/>
       <c r="D49" s="46" t="s">
-        <v>980</v>
-      </c>
-      <c r="E49" s="46" t="s">
         <v>981</v>
+      </c>
+      <c r="E49" s="53" t="s">
+        <v>982</v>
       </c>
       <c r="F49" s="44"/>
       <c r="G49" s="44"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="51" t="s">
+        <v>328</v>
+      </c>
+      <c r="B50" s="28" t="s">
         <v>340</v>
-      </c>
-      <c r="B50" s="28" t="s">
-        <v>338</v>
       </c>
       <c r="C50" s="44"/>
       <c r="D50" s="46" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E50" s="53" t="s">
         <v>983</v>
@@ -14951,14 +14948,14 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="51" t="s">
-        <v>328</v>
+        <v>354</v>
       </c>
       <c r="B51" s="28" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C51" s="44"/>
       <c r="D51" s="46" t="s">
-        <v>982</v>
+        <v>355</v>
       </c>
       <c r="E51" s="53" t="s">
         <v>984</v>
@@ -14968,10 +14965,10 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="51" t="s">
+        <v>328</v>
+      </c>
+      <c r="B52" s="28" t="s">
         <v>354</v>
-      </c>
-      <c r="B52" s="28" t="s">
-        <v>334</v>
       </c>
       <c r="C52" s="44"/>
       <c r="D52" s="46" t="s">
@@ -14985,31 +14982,31 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="51" t="s">
+        <v>334</v>
+      </c>
+      <c r="B53" s="28" t="s">
         <v>328</v>
-      </c>
-      <c r="B53" s="28" t="s">
-        <v>354</v>
       </c>
       <c r="C53" s="44"/>
       <c r="D53" s="46" t="s">
-        <v>355</v>
+        <v>986</v>
       </c>
       <c r="E53" s="53" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="F53" s="44"/>
       <c r="G53" s="44"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="51" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="C54" s="44"/>
       <c r="D54" s="46" t="s">
-        <v>987</v>
+        <v>501</v>
       </c>
       <c r="E54" s="53" t="s">
         <v>988</v>
@@ -15019,31 +15016,31 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="51" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>338</v>
+        <v>352</v>
       </c>
       <c r="C55" s="44"/>
       <c r="D55" s="46" t="s">
-        <v>501</v>
+        <v>989</v>
       </c>
       <c r="E55" s="53" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="F55" s="44"/>
       <c r="G55" s="44"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="51" t="s">
-        <v>328</v>
+        <v>352</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
       <c r="C56" s="44"/>
       <c r="D56" s="46" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="E56" s="53" t="s">
         <v>991</v>
@@ -15053,14 +15050,14 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="51" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="B57" s="28" t="s">
         <v>330</v>
       </c>
       <c r="C57" s="44"/>
       <c r="D57" s="46" t="s">
-        <v>990</v>
+        <v>147</v>
       </c>
       <c r="E57" s="53" t="s">
         <v>992</v>
@@ -15070,14 +15067,14 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="51" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B58" s="28" t="s">
-        <v>330</v>
+        <v>361</v>
       </c>
       <c r="C58" s="44"/>
       <c r="D58" s="46" t="s">
-        <v>147</v>
+        <v>362</v>
       </c>
       <c r="E58" s="53" t="s">
         <v>993</v>
@@ -15087,17 +15084,17 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="51" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="B59" s="28" t="s">
-        <v>361</v>
+        <v>334</v>
       </c>
       <c r="C59" s="44"/>
       <c r="D59" s="46" t="s">
-        <v>362</v>
-      </c>
-      <c r="E59" s="53" t="s">
         <v>994</v>
+      </c>
+      <c r="E59" s="46" t="s">
+        <v>995</v>
       </c>
       <c r="F59" s="44"/>
       <c r="G59" s="44"/>
@@ -15111,24 +15108,24 @@
       </c>
       <c r="C60" s="44"/>
       <c r="D60" s="46" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="E60" s="46" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="F60" s="44"/>
       <c r="G60" s="44"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="51" t="s">
+        <v>328</v>
+      </c>
+      <c r="B61" s="28" t="s">
         <v>340</v>
-      </c>
-      <c r="B61" s="28" t="s">
-        <v>334</v>
       </c>
       <c r="C61" s="44"/>
       <c r="D61" s="46" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E61" s="46" t="s">
         <v>998</v>
@@ -15138,14 +15135,14 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="51" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
       <c r="B62" s="28" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="C62" s="44"/>
       <c r="D62" s="46" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E62" s="46" t="s">
         <v>999</v>
@@ -15155,14 +15152,14 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="51" t="s">
+        <v>328</v>
+      </c>
+      <c r="B63" s="28" t="s">
         <v>340</v>
-      </c>
-      <c r="B63" s="28" t="s">
-        <v>330</v>
       </c>
       <c r="C63" s="44"/>
       <c r="D63" s="46" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E63" s="46" t="s">
         <v>1000</v>
@@ -15172,51 +15169,51 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="51" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C64" s="44"/>
       <c r="D64" s="46" t="s">
-        <v>997</v>
+        <v>1001</v>
       </c>
       <c r="E64" s="46" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
       <c r="F64" s="44"/>
       <c r="G64" s="44"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="51" t="s">
-        <v>330</v>
+        <v>338</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>334</v>
+        <v>363</v>
       </c>
       <c r="C65" s="44"/>
       <c r="D65" s="46" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
       <c r="E65" s="46" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="F65" s="44"/>
       <c r="G65" s="44"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="51" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C66" s="44"/>
       <c r="D66" s="46" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="E66" s="46" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="F66" s="44"/>
       <c r="G66" s="44"/>
@@ -15226,14 +15223,14 @@
         <v>334</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>365</v>
+        <v>328</v>
       </c>
       <c r="C67" s="44"/>
       <c r="D67" s="46" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
       <c r="E67" s="46" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
       <c r="F67" s="44"/>
       <c r="G67" s="44"/>
@@ -15243,11 +15240,11 @@
         <v>334</v>
       </c>
       <c r="B68" s="28" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C68" s="44"/>
       <c r="D68" s="46" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="E68" s="46" t="s">
         <v>1009</v>
@@ -15255,23 +15252,7 @@
       <c r="F68" s="44"/>
       <c r="G68" s="44"/>
     </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="51" t="s">
-        <v>334</v>
-      </c>
-      <c r="B69" s="28" t="s">
-        <v>330</v>
-      </c>
-      <c r="C69" s="44"/>
-      <c r="D69" s="46" t="s">
-        <v>1008</v>
-      </c>
-      <c r="E69" s="46" t="s">
-        <v>1010</v>
-      </c>
-      <c r="F69" s="44"/>
-      <c r="G69" s="44"/>
-    </row>
+    <row r="1048366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -15603,7 +15584,7 @@
       </c>
       <c r="C5" s="44"/>
       <c r="D5" s="46" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="E5" s="46" t="s">
         <v>903</v>
@@ -15630,7 +15611,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="51" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B7" s="28" t="s">
         <v>223</v>
@@ -15647,7 +15628,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="51" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B8" s="28" t="s">
         <v>223</v>
@@ -15664,7 +15645,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="51" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B9" s="28" t="s">
         <v>223</v>
@@ -15681,7 +15662,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="51" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B10" s="28" t="s">
         <v>223</v>
@@ -15698,7 +15679,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="51" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>223</v>
@@ -15715,7 +15696,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="51" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B12" s="28" t="s">
         <v>223</v>
@@ -15749,7 +15730,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="51" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>221</v>
@@ -15766,7 +15747,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="51" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B15" s="28" t="s">
         <v>221</v>
@@ -15783,7 +15764,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="51" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>221</v>
@@ -15800,7 +15781,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="51" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B17" s="28" t="s">
         <v>221</v>
@@ -15817,7 +15798,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="51" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B18" s="28" t="s">
         <v>223</v>
@@ -15834,7 +15815,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="51" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B19" s="28" t="s">
         <v>221</v>
@@ -15853,7 +15834,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="51" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B20" s="28" t="s">
         <v>221</v>
@@ -15870,7 +15851,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="51" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B21" s="28" t="s">
         <v>221</v>
@@ -15887,7 +15868,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="51" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B22" s="28" t="s">
         <v>221</v>
@@ -15904,7 +15885,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="51" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B23" s="28" t="s">
         <v>221</v>
@@ -15921,7 +15902,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="51" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>233</v>
@@ -15955,7 +15936,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="51" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>223</v>
@@ -15979,10 +15960,10 @@
       </c>
       <c r="C27" s="44"/>
       <c r="D27" s="46" t="s">
+        <v>979</v>
+      </c>
+      <c r="E27" s="46" t="s">
         <v>980</v>
-      </c>
-      <c r="E27" s="46" t="s">
-        <v>981</v>
       </c>
       <c r="F27" s="44"/>
       <c r="G27" s="44"/>
@@ -15996,10 +15977,10 @@
       </c>
       <c r="C28" s="44"/>
       <c r="D28" s="46" t="s">
+        <v>986</v>
+      </c>
+      <c r="E28" s="45" t="s">
         <v>987</v>
-      </c>
-      <c r="E28" s="45" t="s">
-        <v>988</v>
       </c>
       <c r="F28" s="44"/>
       <c r="G28" s="44"/>
@@ -16016,7 +15997,7 @@
         <v>355</v>
       </c>
       <c r="E29" s="53" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F29" s="44"/>
       <c r="G29" s="44"/>
@@ -16033,7 +16014,7 @@
         <v>147</v>
       </c>
       <c r="E30" s="53" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F30" s="44"/>
       <c r="G30" s="44"/>
@@ -16047,10 +16028,10 @@
       </c>
       <c r="C31" s="44"/>
       <c r="D31" s="52" t="s">
+        <v>972</v>
+      </c>
+      <c r="E31" s="46" t="s">
         <v>973</v>
-      </c>
-      <c r="E31" s="46" t="s">
-        <v>974</v>
       </c>
       <c r="F31" s="44"/>
       <c r="G31" s="44"/>
@@ -16064,10 +16045,10 @@
       </c>
       <c r="C32" s="44"/>
       <c r="D32" s="46" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E32" s="53" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F32" s="44"/>
       <c r="G32" s="44"/>
@@ -16081,10 +16062,10 @@
       </c>
       <c r="C33" s="44"/>
       <c r="D33" s="46" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="F33" s="44"/>
       <c r="G33" s="44"/>
@@ -16098,10 +16079,10 @@
       </c>
       <c r="C34" s="44"/>
       <c r="D34" s="46" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="E34" s="53" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F34" s="44"/>
       <c r="G34" s="44"/>
@@ -16115,10 +16096,10 @@
       </c>
       <c r="C35" s="44"/>
       <c r="D35" s="46" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="F35" s="44"/>
       <c r="G35" s="44"/>
@@ -16178,563 +16159,563 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B2" s="55" t="s">
         <v>1021</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="C2" s="56" t="s">
         <v>1022</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="D2" s="57" t="s">
+        <v>1020</v>
+      </c>
+      <c r="E2" s="58" t="s">
         <v>1023</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>1021</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B3" s="55" t="s">
         <v>1025</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>1026</v>
       </c>
-      <c r="C3" s="56" t="s">
-        <v>1027</v>
-      </c>
       <c r="D3" s="57" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="E3" s="58" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B4" s="55" t="s">
         <v>1028</v>
       </c>
-      <c r="B4" s="55" t="s">
-        <v>1029</v>
-      </c>
       <c r="C4" s="56" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>1027</v>
+      </c>
+      <c r="E4" s="58" t="s">
         <v>1023</v>
-      </c>
-      <c r="D4" s="57" t="s">
-        <v>1028</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B5" s="55" t="s">
         <v>1030</v>
       </c>
-      <c r="B5" s="55" t="s">
-        <v>1031</v>
-      </c>
       <c r="C5" s="56" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D5" s="57" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="E5" s="58" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B6" s="55" t="s">
         <v>1032</v>
       </c>
-      <c r="B6" s="55" t="s">
-        <v>1033</v>
-      </c>
       <c r="C6" s="59" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D6" s="57" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E6" s="58" t="s">
         <v>1023</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>1032</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B7" s="55" t="s">
         <v>1034</v>
       </c>
-      <c r="B7" s="55" t="s">
-        <v>1035</v>
-      </c>
       <c r="C7" s="59" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D7" s="57" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B8" s="55" t="s">
         <v>1036</v>
       </c>
-      <c r="B8" s="55" t="s">
-        <v>1037</v>
-      </c>
       <c r="C8" s="56" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D8" s="57" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E8" s="58" t="s">
         <v>1023</v>
-      </c>
-      <c r="D8" s="57" t="s">
-        <v>1036</v>
-      </c>
-      <c r="E8" s="58" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B9" s="55" t="s">
         <v>1038</v>
       </c>
-      <c r="B9" s="55" t="s">
-        <v>1039</v>
-      </c>
       <c r="C9" s="56" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D9" s="57" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="E9" s="58" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B10" s="55" t="s">
         <v>1040</v>
       </c>
-      <c r="B10" s="55" t="s">
-        <v>1041</v>
-      </c>
       <c r="C10" s="56" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D10" s="57" t="s">
+        <v>1039</v>
+      </c>
+      <c r="E10" s="58" t="s">
         <v>1023</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>1040</v>
-      </c>
-      <c r="E10" s="58" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B11" s="55" t="s">
         <v>1042</v>
       </c>
-      <c r="B11" s="55" t="s">
-        <v>1043</v>
-      </c>
       <c r="C11" s="56" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D11" s="57" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E11" s="58" t="s">
         <v>1023</v>
-      </c>
-      <c r="D11" s="57" t="s">
-        <v>1042</v>
-      </c>
-      <c r="E11" s="58" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B12" s="55" t="s">
         <v>1044</v>
       </c>
-      <c r="B12" s="55" t="s">
-        <v>1045</v>
-      </c>
       <c r="C12" s="56" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D12" s="57" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B13" s="55" t="s">
         <v>1046</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="C13" s="59" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D13" s="57" t="s">
+        <v>1045</v>
+      </c>
+      <c r="E13" s="60" t="s">
         <v>1047</v>
-      </c>
-      <c r="C13" s="59" t="s">
-        <v>1027</v>
-      </c>
-      <c r="D13" s="57" t="s">
-        <v>1046</v>
-      </c>
-      <c r="E13" s="60" t="s">
-        <v>1048</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B14" s="55" t="s">
         <v>1049</v>
       </c>
-      <c r="B14" s="55" t="s">
-        <v>1050</v>
-      </c>
       <c r="C14" s="59" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D14" s="57" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="E14" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B15" s="55" t="s">
         <v>1051</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="C15" s="59" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D15" s="57" t="s">
         <v>1052</v>
       </c>
-      <c r="C15" s="59" t="s">
-        <v>1027</v>
-      </c>
-      <c r="D15" s="57" t="s">
-        <v>1053</v>
-      </c>
       <c r="E15" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B16" s="55" t="s">
         <v>1054</v>
       </c>
-      <c r="B16" s="55" t="s">
-        <v>1055</v>
-      </c>
       <c r="C16" s="59" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D16" s="57" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="E16" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B17" s="55" t="s">
         <v>1056</v>
       </c>
-      <c r="B17" s="55" t="s">
-        <v>1057</v>
-      </c>
       <c r="C17" s="59" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D17" s="57" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="E17" s="58" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B18" s="55" t="s">
         <v>1058</v>
       </c>
-      <c r="B18" s="55" t="s">
-        <v>1059</v>
-      </c>
       <c r="C18" s="59" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D18" s="57" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="E18" s="58" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B19" s="61" t="s">
         <v>1060</v>
       </c>
-      <c r="B19" s="61" t="s">
+      <c r="C19" s="59" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D19" s="57" t="s">
         <v>1061</v>
       </c>
-      <c r="C19" s="59" t="s">
-        <v>1027</v>
-      </c>
-      <c r="D19" s="57" t="s">
-        <v>1062</v>
-      </c>
       <c r="E19" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B20" s="55" t="s">
         <v>1063</v>
       </c>
-      <c r="B20" s="55" t="s">
-        <v>1064</v>
-      </c>
       <c r="C20" s="56" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D20" s="57" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E20" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B21" s="62" t="s">
         <v>1065</v>
       </c>
-      <c r="B21" s="62" t="s">
+      <c r="C21" s="56" t="s">
         <v>1066</v>
       </c>
-      <c r="C21" s="56" t="s">
+      <c r="D21" s="57" t="s">
+        <v>1064</v>
+      </c>
+      <c r="E21" s="58" t="s">
         <v>1067</v>
-      </c>
-      <c r="D21" s="57" t="s">
-        <v>1065</v>
-      </c>
-      <c r="E21" s="58" t="s">
-        <v>1068</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B22" s="63" t="s">
         <v>1069</v>
       </c>
-      <c r="B22" s="63" t="s">
+      <c r="C22" s="56" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D22" s="57" t="s">
         <v>1070</v>
       </c>
-      <c r="C22" s="56" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D22" s="57" t="s">
-        <v>1071</v>
-      </c>
       <c r="E22" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B23" s="55" t="s">
         <v>1072</v>
       </c>
-      <c r="B23" s="55" t="s">
-        <v>1073</v>
-      </c>
       <c r="C23" s="56" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D23" s="57" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E23" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B24" s="55" t="s">
         <v>1074</v>
       </c>
-      <c r="B24" s="55" t="s">
-        <v>1075</v>
-      </c>
       <c r="C24" s="56" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D24" s="57" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E24" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B25" s="55" t="s">
         <v>1076</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="C25" s="56" t="s">
         <v>1077</v>
       </c>
-      <c r="C25" s="56" t="s">
-        <v>1078</v>
-      </c>
       <c r="D25" s="57" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="E25" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B26" s="64" t="s">
         <v>1079</v>
       </c>
-      <c r="B26" s="64" t="s">
+      <c r="C26" s="56" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D26" s="65" t="s">
         <v>1080</v>
       </c>
-      <c r="C26" s="56" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D26" s="65" t="s">
-        <v>1081</v>
-      </c>
       <c r="E26" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B27" s="64" t="s">
         <v>1082</v>
       </c>
-      <c r="B27" s="64" t="s">
+      <c r="C27" s="66" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D27" s="65" t="s">
         <v>1083</v>
       </c>
-      <c r="C27" s="66" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D27" s="65" t="s">
-        <v>1084</v>
-      </c>
       <c r="E27" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>1084</v>
+      </c>
+      <c r="B28" s="64" t="s">
         <v>1085</v>
       </c>
-      <c r="B28" s="64" t="s">
+      <c r="C28" s="66" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D28" s="65" t="s">
         <v>1086</v>
       </c>
-      <c r="C28" s="66" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D28" s="65" t="s">
-        <v>1087</v>
-      </c>
       <c r="E28" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>1087</v>
+      </c>
+      <c r="B29" s="64" t="s">
         <v>1088</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="C29" s="66" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D29" s="65" t="s">
         <v>1089</v>
       </c>
-      <c r="C29" s="66" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D29" s="65" t="s">
-        <v>1090</v>
-      </c>
       <c r="E29" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>1090</v>
+      </c>
+      <c r="B30" s="64" t="s">
         <v>1091</v>
       </c>
-      <c r="B30" s="64" t="s">
+      <c r="C30" s="56" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D30" s="65" t="s">
         <v>1092</v>
       </c>
-      <c r="C30" s="56" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D30" s="65" t="s">
-        <v>1093</v>
-      </c>
       <c r="E30" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>1093</v>
+      </c>
+      <c r="B31" s="64" t="s">
         <v>1094</v>
       </c>
-      <c r="B31" s="64" t="s">
+      <c r="C31" s="66" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D31" s="65" t="s">
         <v>1095</v>
       </c>
-      <c r="C31" s="66" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D31" s="65" t="s">
-        <v>1096</v>
-      </c>
       <c r="E31" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B32" s="55" t="s">
         <v>1097</v>
       </c>
-      <c r="B32" s="55" t="s">
-        <v>1098</v>
-      </c>
       <c r="C32" s="56" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D32" s="57" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E32" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B33" s="61" t="s">
         <v>1099</v>
       </c>
-      <c r="B33" s="61" t="s">
+      <c r="C33" s="59" t="s">
         <v>1100</v>
       </c>
-      <c r="C33" s="59" t="s">
-        <v>1101</v>
-      </c>
       <c r="D33" s="65" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="E33" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B34" s="61" t="s">
         <v>1102</v>
       </c>
-      <c r="B34" s="61" t="s">
-        <v>1103</v>
-      </c>
       <c r="C34" s="59" t="s">
+        <v>1100</v>
+      </c>
+      <c r="D34" s="57" t="s">
         <v>1101</v>
       </c>
-      <c r="D34" s="57" t="s">
-        <v>1102</v>
-      </c>
       <c r="E34" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
   </sheetData>
@@ -16795,274 +16776,274 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B2" s="55" t="s">
         <v>1104</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>1105</v>
       </c>
       <c r="C2" s="56"/>
       <c r="D2" s="57" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="E2" s="67" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B3" s="55" t="s">
         <v>1106</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="C3" s="56" t="s">
         <v>1107</v>
       </c>
-      <c r="C3" s="56" t="s">
-        <v>1108</v>
-      </c>
       <c r="D3" s="57" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E3" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B4" s="55" t="s">
         <v>1109</v>
-      </c>
-      <c r="B4" s="55" t="s">
-        <v>1110</v>
       </c>
       <c r="C4" s="56"/>
       <c r="D4" s="57" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B5" s="55" t="s">
         <v>1111</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>1112</v>
       </c>
       <c r="C5" s="56"/>
       <c r="D5" s="57" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E5" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B6" s="55" t="s">
         <v>1113</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>1114</v>
       </c>
       <c r="C6" s="56"/>
       <c r="D6" s="57" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B7" s="55" t="s">
         <v>1115</v>
-      </c>
-      <c r="B7" s="55" t="s">
-        <v>1116</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="57" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B8" s="55" t="s">
         <v>1117</v>
-      </c>
-      <c r="B8" s="55" t="s">
-        <v>1118</v>
       </c>
       <c r="C8" s="56"/>
       <c r="D8" s="57" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B9" s="55" t="s">
         <v>1119</v>
-      </c>
-      <c r="B9" s="55" t="s">
-        <v>1120</v>
       </c>
       <c r="C9" s="56"/>
       <c r="D9" s="57" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="E9" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B10" s="55" t="s">
         <v>1121</v>
-      </c>
-      <c r="B10" s="55" t="s">
-        <v>1122</v>
       </c>
       <c r="C10" s="56"/>
       <c r="D10" s="57" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B11" s="55" t="s">
         <v>1123</v>
-      </c>
-      <c r="B11" s="55" t="s">
-        <v>1124</v>
       </c>
       <c r="C11" s="56"/>
       <c r="D11" s="57" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="E11" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B12" s="55" t="s">
         <v>1125</v>
-      </c>
-      <c r="B12" s="55" t="s">
-        <v>1126</v>
       </c>
       <c r="C12" s="56"/>
       <c r="D12" s="57" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="E12" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B13" s="55" t="s">
         <v>1127</v>
-      </c>
-      <c r="B13" s="55" t="s">
-        <v>1128</v>
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="57" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="E13" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B14" s="55" t="s">
         <v>1129</v>
-      </c>
-      <c r="B14" s="55" t="s">
-        <v>1130</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="57" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="E14" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B15" s="55" t="s">
         <v>1131</v>
-      </c>
-      <c r="B15" s="55" t="s">
-        <v>1132</v>
       </c>
       <c r="C15" s="56"/>
       <c r="D15" s="57" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E15" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B16" s="55" t="s">
         <v>1133</v>
-      </c>
-      <c r="B16" s="55" t="s">
-        <v>1134</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="57" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="E16" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B17" s="55" t="s">
         <v>1135</v>
-      </c>
-      <c r="B17" s="55" t="s">
-        <v>1136</v>
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="57" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="E17" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B18" s="55" t="s">
         <v>1137</v>
-      </c>
-      <c r="B18" s="55" t="s">
-        <v>1138</v>
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="57" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="E18" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B19" s="55" t="s">
         <v>1139</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>1140</v>
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="57" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="E19" s="60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improvements in costs and post processing files
</commit_message>
<xml_diff>
--- a/SEPIA/SEPIA_config.xlsx
+++ b/SEPIA/SEPIA_config.xlsx
@@ -2198,7 +2198,7 @@
     <t xml:space="preserve">Oil</t>
   </si>
   <si>
-    <t xml:space="preserve">Heat energy output from centralised resistive heaters</t>
+    <t xml:space="preserve">Heat energy output from centralised electric boilers</t>
   </si>
   <si>
     <t xml:space="preserve">prbchresh</t>
@@ -2207,7 +2207,7 @@
     <t xml:space="preserve">prbchreshh</t>
   </si>
   <si>
-    <t xml:space="preserve">Losses from centralised resistive heaters</t>
+    <t xml:space="preserve">Losses from centralised electric boilers</t>
   </si>
   <si>
     <t xml:space="preserve">losselchh</t>
@@ -2774,35 +2774,7 @@
     <t xml:space="preserve">presvapcfdhs</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3F3F76"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Residential </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3F3F76"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ambient </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3F3F76"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">rural  heat pumps</t>
-    </r>
+    <t xml:space="preserve">Residential  ambient rural  heat pumps</t>
   </si>
   <si>
     <t xml:space="preserve">prespaccfres</t>
@@ -2811,35 +2783,7 @@
     <t xml:space="preserve">prespaccfra</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3F3F76"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Residential </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3F3F76"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ambient </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF3F3F76"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">urban heat pumps</t>
-    </r>
+    <t xml:space="preserve">Residential  ambient urban heat pumps</t>
   </si>
   <si>
     <t xml:space="preserve">prespaccfraa</t>
@@ -4550,7 +4494,7 @@
     <numFmt numFmtId="168" formatCode="0.0000"/>
     <numFmt numFmtId="169" formatCode="0%"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4624,12 +4568,6 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -5130,15 +5068,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="22" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5146,7 +5084,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5158,11 +5096,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5170,7 +5108,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5194,11 +5132,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -5588,10 +5526,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D4" activeCellId="1" sqref="193:193 D4"/>
+      <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.91"/>
@@ -6196,10 +6134,10 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="193:193 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -6844,10 +6782,10 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="1" sqref="193:193 F31"/>
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -7498,10 +7436,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C4" activeCellId="1" sqref="193:193 C4"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.28"/>
@@ -7682,14 +7620,14 @@
   <dimension ref="A1:T106"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D77" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
-      <selection pane="bottomRight" activeCell="J86" activeCellId="1" sqref="193:193 J86"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="J86" activeCellId="0" sqref="J86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.36"/>
@@ -10302,12 +10240,12 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A193" activeCellId="0" sqref="193:193"/>
+      <selection pane="bottomLeft" activeCell="D88" activeCellId="0" sqref="D88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -16059,10 +15997,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A71" activeCellId="1" sqref="193:193 A71"/>
+      <selection pane="bottomLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -17582,10 +17520,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B37" activeCellId="1" sqref="193:193 B37"/>
+      <selection pane="bottomLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="46" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -18478,10 +18416,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B26" activeCellId="1" sqref="193:193 B26"/>
+      <selection pane="bottomLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -19095,10 +19033,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B2" activeCellId="1" sqref="193:193 B2"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -19420,10 +19358,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ9" activeCellId="1" sqref="193:193 AQ9"/>
+      <selection pane="bottomRight" activeCell="AQ9" activeCellId="0" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.27"/>

</xml_diff>

<commit_message>
New changes in scripts
</commit_message>
<xml_diff>
--- a/SEPIA/SEPIA_config.xlsx
+++ b/SEPIA/SEPIA_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" state="visible" r:id="rId2"/>
@@ -1331,7 +1331,7 @@
     <t xml:space="preserve">CRF1A1B-CRF1A1C</t>
   </si>
   <si>
-    <t xml:space="preserve">Fuel combustion - industry</t>
+    <t xml:space="preserve">Fuel usage - industry</t>
   </si>
   <si>
     <t xml:space="preserve">CRF1A2</t>
@@ -5560,7 +5560,7 @@
       <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.91"/>
@@ -5686,7 +5686,7 @@
       <c r="B11" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="2" t="b">
+      <c r="C11" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5698,7 +5698,7 @@
       <c r="B12" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="2" t="b">
+      <c r="C12" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5710,7 +5710,7 @@
       <c r="B13" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="2" t="b">
+      <c r="C13" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5722,7 +5722,7 @@
       <c r="B14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="2" t="b">
+      <c r="C14" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5734,7 +5734,7 @@
       <c r="B15" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="2" t="b">
+      <c r="C15" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5746,7 +5746,7 @@
       <c r="B16" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="2" t="b">
+      <c r="C16" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5758,7 +5758,7 @@
       <c r="B17" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="2" t="b">
+      <c r="C17" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5770,7 +5770,7 @@
       <c r="B18" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="2" t="b">
+      <c r="C18" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5782,7 +5782,7 @@
       <c r="B19" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="2" t="b">
+      <c r="C19" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5794,7 +5794,7 @@
       <c r="B20" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="2" t="b">
+      <c r="C20" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5806,7 +5806,7 @@
       <c r="B21" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="2" t="b">
+      <c r="C21" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5818,7 +5818,7 @@
       <c r="B22" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="2" t="b">
+      <c r="C22" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5830,7 +5830,7 @@
       <c r="B23" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="2" t="b">
+      <c r="C23" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5842,7 +5842,7 @@
       <c r="B24" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="2" t="b">
+      <c r="C24" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5854,7 +5854,7 @@
       <c r="B25" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="2" t="b">
+      <c r="C25" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5866,7 +5866,7 @@
       <c r="B26" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="2" t="b">
+      <c r="C26" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5934,7 +5934,7 @@
       <c r="B32" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="2" t="b">
+      <c r="C32" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5946,7 +5946,7 @@
       <c r="B33" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="2" t="b">
+      <c r="C33" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5958,7 +5958,7 @@
       <c r="B34" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="2" t="b">
+      <c r="C34" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6082,7 +6082,7 @@
       <c r="B45" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="2" t="b">
+      <c r="C45" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6094,7 +6094,7 @@
       <c r="B46" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="2" t="b">
+      <c r="C46" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -6168,7 +6168,7 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -6816,7 +6816,7 @@
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -7470,7 +7470,7 @@
       <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.28"/>
@@ -7650,15 +7650,15 @@
   </sheetPr>
   <dimension ref="A1:T108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D65" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="D67" activeCellId="0" sqref="D67"/>
+      <selection pane="bottomLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
+      <selection pane="bottomRight" activeCell="C73" activeCellId="0" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.36"/>
@@ -10298,13 +10298,13 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E304" activeCellId="0" sqref="E304"/>
+      <selection pane="bottomLeft" activeCell="C263" activeCellId="0" sqref="C263"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -16070,12 +16070,12 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E75" activeCellId="0" sqref="E75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -17609,12 +17609,12 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -18527,7 +18527,7 @@
       <selection pane="bottomLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -19144,7 +19144,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -19469,7 +19469,7 @@
       <selection pane="bottomRight" activeCell="AQ9" activeCellId="0" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.27"/>

</xml_diff>

<commit_message>
Changing 2020 planning horizon to myopic, correcting pre-installed capacities and generation pattern for nuclear and improvements in post processing
</commit_message>
<xml_diff>
--- a/SEPIA/SEPIA_config.xlsx
+++ b/SEPIA/SEPIA_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" state="visible" r:id="rId2"/>
@@ -432,7 +432,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="1288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="1289">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -3516,6 +3516,9 @@
   </si>
   <si>
     <t xml:space="preserve">emmindatmbm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BECCUS</t>
   </si>
   <si>
     <t xml:space="preserve">emmindbeccs</t>
@@ -5560,7 +5563,7 @@
       <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.91"/>
@@ -5686,7 +5689,7 @@
       <c r="B11" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="0" t="b">
+      <c r="C11" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5698,7 +5701,7 @@
       <c r="B12" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="0" t="b">
+      <c r="C12" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5710,7 +5713,7 @@
       <c r="B13" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="0" t="b">
+      <c r="C13" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5722,7 +5725,7 @@
       <c r="B14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="0" t="b">
+      <c r="C14" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5734,7 +5737,7 @@
       <c r="B15" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="0" t="b">
+      <c r="C15" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5746,7 +5749,7 @@
       <c r="B16" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="0" t="b">
+      <c r="C16" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5758,7 +5761,7 @@
       <c r="B17" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="0" t="b">
+      <c r="C17" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5770,7 +5773,7 @@
       <c r="B18" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="0" t="b">
+      <c r="C18" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5782,7 +5785,7 @@
       <c r="B19" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="0" t="b">
+      <c r="C19" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5794,7 +5797,7 @@
       <c r="B20" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="0" t="b">
+      <c r="C20" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5806,7 +5809,7 @@
       <c r="B21" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="0" t="b">
+      <c r="C21" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5818,7 +5821,7 @@
       <c r="B22" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="0" t="b">
+      <c r="C22" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5830,7 +5833,7 @@
       <c r="B23" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="0" t="b">
+      <c r="C23" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5842,7 +5845,7 @@
       <c r="B24" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="0" t="b">
+      <c r="C24" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5854,7 +5857,7 @@
       <c r="B25" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="0" t="b">
+      <c r="C25" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5866,7 +5869,7 @@
       <c r="B26" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="0" t="b">
+      <c r="C26" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -5934,7 +5937,7 @@
       <c r="B32" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="0" t="b">
+      <c r="C32" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5946,7 +5949,7 @@
       <c r="B33" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="0" t="b">
+      <c r="C33" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -5958,7 +5961,7 @@
       <c r="B34" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="0" t="b">
+      <c r="C34" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6082,7 +6085,7 @@
       <c r="B45" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="0" t="b">
+      <c r="C45" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6094,7 +6097,7 @@
       <c r="B46" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="C46" s="0" t="b">
+      <c r="C46" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -6168,11 +6171,11 @@
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>2020</v>
@@ -6189,7 +6192,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>10</v>
@@ -6204,12 +6207,12 @@
         <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1206</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -6224,12 +6227,12 @@
         <v>0</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>1208</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.6</v>
@@ -6244,12 +6247,12 @@
         <v>0.6</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -6264,12 +6267,12 @@
         <v>0</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1.28</v>
@@ -6284,12 +6287,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>47</v>
@@ -6304,12 +6307,12 @@
         <v>40</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>20</v>
@@ -6324,12 +6327,12 @@
         <v>0</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -6344,12 +6347,12 @@
         <v>0</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0</v>
@@ -6364,12 +6367,12 @@
         <v>0</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -6384,12 +6387,12 @@
         <v>0</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -6404,12 +6407,12 @@
         <v>0</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -6424,12 +6427,12 @@
         <v>0</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>8</v>
@@ -6444,12 +6447,12 @@
         <v>0</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>16</v>
@@ -6464,12 +6467,12 @@
         <v>16</v>
       </c>
       <c r="F15" s="26" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>19</v>
@@ -6484,12 +6487,12 @@
         <v>19</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>31</v>
@@ -6504,12 +6507,12 @@
         <v>20</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -6524,12 +6527,12 @@
         <v>0</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -6544,12 +6547,12 @@
         <v>0</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -6564,12 +6567,12 @@
         <v>0</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>107</v>
@@ -6584,12 +6587,12 @@
         <v>107</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1000</v>
@@ -6604,12 +6607,12 @@
         <v>1000</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>43</v>
@@ -6624,12 +6627,12 @@
         <v>43</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -6644,12 +6647,12 @@
         <v>0</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>68</v>
@@ -6664,12 +6667,12 @@
         <v>68</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -6684,12 +6687,12 @@
         <v>0</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -6704,12 +6707,12 @@
         <v>0</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
@@ -6724,12 +6727,12 @@
         <v>0</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>351</v>
@@ -6744,12 +6747,12 @@
         <v>341</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">SUM(B2:B29)</f>
@@ -6816,11 +6819,11 @@
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>2020</v>
@@ -6837,7 +6840,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>6.5</v>
@@ -6852,12 +6855,12 @@
         <v>4</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1207</v>
+        <v>1208</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0</v>
@@ -6872,12 +6875,12 @@
         <v>0</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0</v>
@@ -6892,12 +6895,12 @@
         <v>0</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0</v>
@@ -6912,12 +6915,12 @@
         <v>0</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1.36</v>
@@ -6932,12 +6935,12 @@
         <v>1</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>38</v>
@@ -6952,12 +6955,12 @@
         <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>42</v>
@@ -6972,12 +6975,12 @@
         <v>0</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -6992,12 +6995,12 @@
         <v>0</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>1</v>
@@ -7012,12 +7015,12 @@
         <v>1</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0</v>
@@ -7032,12 +7035,12 @@
         <v>0</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -7052,12 +7055,12 @@
         <v>0</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>9</v>
@@ -7072,12 +7075,12 @@
         <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>8</v>
@@ -7092,12 +7095,12 @@
         <v>8</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>13</v>
@@ -7112,12 +7115,12 @@
         <v>13</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>0</v>
@@ -7132,12 +7135,12 @@
         <v>0</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>60</v>
@@ -7152,12 +7155,12 @@
         <v>60</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0</v>
@@ -7172,12 +7175,12 @@
         <v>0</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>0</v>
@@ -7192,12 +7195,12 @@
         <v>0</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>0</v>
@@ -7212,12 +7215,12 @@
         <v>0</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>12</v>
@@ -7232,12 +7235,12 @@
         <v>12</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>1076</v>
@@ -7252,12 +7255,12 @@
         <v>1000</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>11</v>
@@ -7272,12 +7275,12 @@
         <v>0</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>0</v>
@@ -7292,12 +7295,12 @@
         <v>0</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>40</v>
@@ -7312,12 +7315,12 @@
         <v>40</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -7332,12 +7335,12 @@
         <v>0</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -7352,12 +7355,12 @@
         <v>0</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>2.4</v>
@@ -7372,12 +7375,12 @@
         <v>2.4</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>616</v>
@@ -7392,12 +7395,12 @@
         <v>600</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="B30" s="0" t="n">
         <f aca="false">SUM(B2:B29)</f>
@@ -7470,7 +7473,7 @@
       <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.28"/>
@@ -7650,15 +7653,15 @@
   </sheetPr>
   <dimension ref="A1:T108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D65" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D80" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
+      <selection pane="bottomLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
       <selection pane="bottomRight" activeCell="C73" activeCellId="0" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.36"/>
@@ -10299,12 +10302,12 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C263" activeCellId="0" sqref="C263"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -16069,13 +16072,13 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E75" activeCellId="0" sqref="E75"/>
+      <selection pane="bottomLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -16840,7 +16843,7 @@
         <v>333</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="C44" s="43"/>
       <c r="D44" s="44" t="s">
@@ -16854,17 +16857,17 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="49" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="B45" s="27" t="s">
         <v>335</v>
       </c>
       <c r="C45" s="43"/>
       <c r="D45" s="44" t="s">
-        <v>362</v>
+        <v>1028</v>
       </c>
       <c r="E45" s="44" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="F45" s="43"/>
       <c r="G45" s="43"/>
@@ -16878,10 +16881,10 @@
       </c>
       <c r="C46" s="43"/>
       <c r="D46" s="44" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="E46" s="44" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="F46" s="43"/>
       <c r="G46" s="43"/>
@@ -16895,10 +16898,10 @@
       </c>
       <c r="C47" s="43"/>
       <c r="D47" s="44" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="E47" s="44" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="F47" s="43"/>
       <c r="G47" s="43"/>
@@ -16912,10 +16915,10 @@
       </c>
       <c r="C48" s="43"/>
       <c r="D48" s="44" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="E48" s="44" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="F48" s="43"/>
       <c r="G48" s="43"/>
@@ -16929,10 +16932,10 @@
       </c>
       <c r="C49" s="43"/>
       <c r="D49" s="44" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="E49" s="51" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="F49" s="43"/>
       <c r="G49" s="43"/>
@@ -16946,10 +16949,10 @@
       </c>
       <c r="C50" s="43"/>
       <c r="D50" s="44" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="E50" s="51" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="F50" s="43"/>
       <c r="G50" s="43"/>
@@ -16966,7 +16969,7 @@
         <v>365</v>
       </c>
       <c r="E51" s="51" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="F51" s="43"/>
       <c r="G51" s="43"/>
@@ -16983,7 +16986,7 @@
         <v>365</v>
       </c>
       <c r="E52" s="51" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="F52" s="43"/>
       <c r="G52" s="43"/>
@@ -16997,10 +17000,10 @@
       </c>
       <c r="C53" s="43"/>
       <c r="D53" s="44" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="E53" s="51" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="F53" s="43"/>
       <c r="G53" s="43"/>
@@ -17016,10 +17019,10 @@
         <v>398</v>
       </c>
       <c r="D54" s="44" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="E54" s="51" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F54" s="43"/>
       <c r="G54" s="43"/>
@@ -17033,10 +17036,10 @@
       </c>
       <c r="C55" s="43"/>
       <c r="D55" s="44" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="E55" s="51" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="F55" s="43"/>
       <c r="G55" s="43"/>
@@ -17050,10 +17053,10 @@
       </c>
       <c r="C56" s="43"/>
       <c r="D56" s="44" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="E56" s="51" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="F56" s="43"/>
       <c r="G56" s="43"/>
@@ -17070,7 +17073,7 @@
         <v>523</v>
       </c>
       <c r="E57" s="51" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="F57" s="43"/>
       <c r="G57" s="43"/>
@@ -17080,31 +17083,31 @@
         <v>333</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="C58" s="43"/>
       <c r="D58" s="44" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="E58" s="51" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="F58" s="43"/>
       <c r="G58" s="43"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="49" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="B59" s="27" t="s">
         <v>335</v>
       </c>
       <c r="C59" s="43"/>
       <c r="D59" s="44" t="s">
-        <v>1046</v>
+        <v>1028</v>
       </c>
       <c r="E59" s="51" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="F59" s="43"/>
       <c r="G59" s="43"/>
@@ -17121,7 +17124,7 @@
         <v>371</v>
       </c>
       <c r="E60" s="51" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="F60" s="43"/>
       <c r="G60" s="43"/>
@@ -17138,7 +17141,7 @@
         <v>373</v>
       </c>
       <c r="E61" s="51" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="F61" s="43"/>
       <c r="G61" s="43"/>
@@ -17152,10 +17155,10 @@
       </c>
       <c r="C62" s="43"/>
       <c r="D62" s="44" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="E62" s="44" t="s">
-        <v>1052</v>
+        <v>1053</v>
       </c>
       <c r="F62" s="43"/>
       <c r="G62" s="43"/>
@@ -17169,10 +17172,10 @@
       </c>
       <c r="C63" s="43"/>
       <c r="D63" s="44" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="E63" s="44" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F63" s="43"/>
       <c r="G63" s="43"/>
@@ -17186,10 +17189,10 @@
       </c>
       <c r="C64" s="43"/>
       <c r="D64" s="44" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E64" s="44" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="F64" s="43"/>
       <c r="G64" s="43"/>
@@ -17203,10 +17206,10 @@
       </c>
       <c r="C65" s="43"/>
       <c r="D65" s="44" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E65" s="44" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="F65" s="43"/>
       <c r="G65" s="43"/>
@@ -17220,10 +17223,10 @@
       </c>
       <c r="C66" s="43"/>
       <c r="D66" s="44" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E66" s="44" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="F66" s="43"/>
       <c r="G66" s="43"/>
@@ -17237,10 +17240,10 @@
       </c>
       <c r="C67" s="43"/>
       <c r="D67" s="44" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E67" s="44" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="F67" s="43"/>
       <c r="G67" s="43"/>
@@ -17254,10 +17257,10 @@
       </c>
       <c r="C68" s="43"/>
       <c r="D68" s="44" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="E68" s="44" t="s">
-        <v>1060</v>
+        <v>1061</v>
       </c>
       <c r="F68" s="43"/>
       <c r="G68" s="43"/>
@@ -17271,10 +17274,10 @@
       </c>
       <c r="C69" s="43"/>
       <c r="D69" s="44" t="s">
-        <v>1061</v>
+        <v>1062</v>
       </c>
       <c r="E69" s="44" t="s">
-        <v>1062</v>
+        <v>1063</v>
       </c>
       <c r="F69" s="43"/>
       <c r="G69" s="43"/>
@@ -17288,10 +17291,10 @@
       </c>
       <c r="C70" s="43"/>
       <c r="D70" s="44" t="s">
-        <v>1063</v>
+        <v>1064</v>
       </c>
       <c r="E70" s="44" t="s">
-        <v>1064</v>
+        <v>1065</v>
       </c>
       <c r="F70" s="43"/>
       <c r="G70" s="43"/>
@@ -17305,10 +17308,10 @@
       </c>
       <c r="C71" s="43"/>
       <c r="D71" s="44" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="E71" s="44" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="F71" s="43"/>
       <c r="G71" s="43"/>
@@ -17322,10 +17325,10 @@
       </c>
       <c r="C72" s="43"/>
       <c r="D72" s="44" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="E72" s="44" t="s">
-        <v>1067</v>
+        <v>1068</v>
       </c>
       <c r="F72" s="43"/>
       <c r="G72" s="43"/>
@@ -17342,7 +17345,7 @@
         <v>381</v>
       </c>
       <c r="E73" s="50" t="s">
-        <v>1068</v>
+        <v>1069</v>
       </c>
       <c r="F73" s="43"/>
       <c r="G73" s="43"/>
@@ -17356,10 +17359,10 @@
       </c>
       <c r="C74" s="43"/>
       <c r="D74" s="50" t="s">
-        <v>1069</v>
+        <v>1070</v>
       </c>
       <c r="E74" s="50" t="s">
-        <v>1070</v>
+        <v>1071</v>
       </c>
       <c r="F74" s="43"/>
       <c r="G74" s="43"/>
@@ -17373,10 +17376,10 @@
       </c>
       <c r="C75" s="43"/>
       <c r="D75" s="50" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="E75" s="50" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="F75" s="43"/>
       <c r="G75" s="43"/>
@@ -17609,12 +17612,12 @@
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E51" activeCellId="0" sqref="E51"/>
+      <selection pane="bottomLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -17708,7 +17711,7 @@
       </c>
       <c r="C5" s="43"/>
       <c r="D5" s="44" t="s">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="E5" s="44" t="s">
         <v>957</v>
@@ -17735,7 +17738,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="49" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>227</v>
@@ -17752,7 +17755,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="49" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>227</v>
@@ -17769,7 +17772,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>227</v>
@@ -17786,7 +17789,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>227</v>
@@ -17803,7 +17806,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>227</v>
@@ -17820,7 +17823,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>227</v>
@@ -17854,7 +17857,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>225</v>
@@ -17871,7 +17874,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>225</v>
@@ -17888,7 +17891,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>225</v>
@@ -17905,7 +17908,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>225</v>
@@ -17922,7 +17925,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="49" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>227</v>
@@ -17939,7 +17942,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="49" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>225</v>
@@ -17958,7 +17961,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="49" t="s">
-        <v>1077</v>
+        <v>1078</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>225</v>
@@ -17975,7 +17978,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="49" t="s">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>225</v>
@@ -17992,7 +17995,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="49" t="s">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>225</v>
@@ -18009,7 +18012,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="49" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>225</v>
@@ -18026,7 +18029,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="49" t="s">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>234</v>
@@ -18060,7 +18063,7 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="49" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B26" s="27" t="s">
         <v>227</v>
@@ -18084,10 +18087,10 @@
       </c>
       <c r="C27" s="43"/>
       <c r="D27" s="44" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="F27" s="43"/>
       <c r="G27" s="43"/>
@@ -18101,10 +18104,10 @@
       </c>
       <c r="C28" s="43"/>
       <c r="D28" s="44" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="E28" s="45" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="F28" s="43"/>
       <c r="G28" s="43"/>
@@ -18121,7 +18124,7 @@
         <v>365</v>
       </c>
       <c r="E29" s="51" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="F29" s="43"/>
       <c r="G29" s="43"/>
@@ -18135,10 +18138,10 @@
       </c>
       <c r="C30" s="43"/>
       <c r="D30" s="44" t="s">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="E30" s="51" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="F30" s="43"/>
       <c r="G30" s="43"/>
@@ -18155,17 +18158,17 @@
         <v>371</v>
       </c>
       <c r="E31" s="51" t="s">
-        <v>1049</v>
+        <v>1050</v>
       </c>
       <c r="F31" s="43"/>
       <c r="G31" s="43"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="52" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="B32" s="52" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="C32" s="43"/>
       <c r="D32" s="50" t="s">
@@ -18186,61 +18189,61 @@
       </c>
       <c r="C33" s="43"/>
       <c r="D33" s="44" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="E33" s="51" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="F33" s="43"/>
       <c r="G33" s="43"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="49" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="C34" s="43"/>
       <c r="D34" s="44" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="E34" s="44" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="F34" s="43"/>
       <c r="G34" s="43"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="49" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="C35" s="43"/>
       <c r="D35" s="44" t="s">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="E35" s="51" t="s">
-        <v>1048</v>
+        <v>1049</v>
       </c>
       <c r="F35" s="43"/>
       <c r="G35" s="43"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="49" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="C36" s="43"/>
       <c r="D36" s="44" t="s">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="E36" s="44" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="F36" s="43"/>
       <c r="G36" s="43"/>
@@ -18254,17 +18257,17 @@
       </c>
       <c r="C37" s="43"/>
       <c r="D37" s="44" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="E37" s="44" t="s">
-        <v>1053</v>
+        <v>1054</v>
       </c>
       <c r="F37" s="43"/>
       <c r="G37" s="43"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="49" t="s">
-        <v>1076</v>
+        <v>1077</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>345</v>
@@ -18298,7 +18301,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>345</v>
@@ -18332,7 +18335,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B42" s="27" t="s">
         <v>345</v>
@@ -18366,7 +18369,7 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B44" s="27" t="s">
         <v>345</v>
@@ -18400,7 +18403,7 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="49" t="s">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B46" s="27" t="s">
         <v>345</v>
@@ -18434,17 +18437,17 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="49" t="s">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B48" s="27" t="s">
         <v>345</v>
       </c>
       <c r="C48" s="43"/>
       <c r="D48" s="44" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="E48" s="44" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="F48" s="43"/>
       <c r="G48" s="43"/>
@@ -18458,10 +18461,10 @@
       </c>
       <c r="C49" s="43"/>
       <c r="D49" s="44" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="E49" s="44" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="F49" s="43"/>
       <c r="G49" s="43"/>
@@ -18475,10 +18478,10 @@
       </c>
       <c r="C50" s="43"/>
       <c r="D50" s="44" t="s">
-        <v>1065</v>
+        <v>1066</v>
       </c>
       <c r="E50" s="44" t="s">
-        <v>1066</v>
+        <v>1067</v>
       </c>
       <c r="F50" s="43"/>
       <c r="G50" s="43"/>
@@ -18492,10 +18495,10 @@
       </c>
       <c r="C51" s="43"/>
       <c r="D51" s="44" t="s">
-        <v>1071</v>
+        <v>1072</v>
       </c>
       <c r="E51" s="50" t="s">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="F51" s="43"/>
       <c r="G51" s="43"/>
@@ -18527,7 +18530,7 @@
       <selection pane="bottomLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -18554,563 +18557,563 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1084</v>
+        <v>1085</v>
       </c>
       <c r="B2" s="53" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D2" s="55" t="s">
         <v>1085</v>
       </c>
-      <c r="C2" s="54" t="s">
-        <v>1086</v>
-      </c>
-      <c r="D2" s="55" t="s">
-        <v>1084</v>
-      </c>
       <c r="E2" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E3" s="56" t="s">
         <v>1088</v>
-      </c>
-      <c r="B3" s="53" t="s">
-        <v>1089</v>
-      </c>
-      <c r="C3" s="54" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>1088</v>
-      </c>
-      <c r="E3" s="56" t="s">
-        <v>1087</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1091</v>
+        <v>1092</v>
       </c>
       <c r="B4" s="53" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D4" s="55" t="s">
         <v>1092</v>
       </c>
-      <c r="C4" s="54" t="s">
-        <v>1086</v>
-      </c>
-      <c r="D4" s="55" t="s">
-        <v>1091</v>
-      </c>
       <c r="E4" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="B5" s="53" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D5" s="55" t="s">
         <v>1094</v>
       </c>
-      <c r="C5" s="54" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D5" s="55" t="s">
-        <v>1093</v>
-      </c>
       <c r="E5" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B6" s="53" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C6" s="57" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D6" s="55" t="s">
         <v>1096</v>
       </c>
-      <c r="C6" s="57" t="s">
-        <v>1086</v>
-      </c>
-      <c r="D6" s="55" t="s">
-        <v>1095</v>
-      </c>
       <c r="E6" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B7" s="53" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C7" s="57" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D7" s="55" t="s">
         <v>1098</v>
       </c>
-      <c r="C7" s="57" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D7" s="55" t="s">
-        <v>1097</v>
-      </c>
       <c r="E7" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B8" s="53" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D8" s="55" t="s">
         <v>1100</v>
       </c>
-      <c r="C8" s="54" t="s">
-        <v>1086</v>
-      </c>
-      <c r="D8" s="55" t="s">
-        <v>1099</v>
-      </c>
       <c r="E8" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B9" s="53" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D9" s="55" t="s">
         <v>1102</v>
       </c>
-      <c r="C9" s="54" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D9" s="55" t="s">
-        <v>1101</v>
-      </c>
       <c r="E9" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B10" s="53" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D10" s="55" t="s">
         <v>1104</v>
       </c>
-      <c r="C10" s="54" t="s">
-        <v>1086</v>
-      </c>
-      <c r="D10" s="55" t="s">
-        <v>1103</v>
-      </c>
       <c r="E10" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="B11" s="53" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>1087</v>
+      </c>
+      <c r="D11" s="55" t="s">
         <v>1106</v>
       </c>
-      <c r="C11" s="54" t="s">
-        <v>1086</v>
-      </c>
-      <c r="D11" s="55" t="s">
-        <v>1105</v>
-      </c>
       <c r="E11" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1107</v>
+        <v>1108</v>
       </c>
       <c r="B12" s="53" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D12" s="55" t="s">
         <v>1108</v>
       </c>
-      <c r="C12" s="54" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D12" s="55" t="s">
-        <v>1107</v>
-      </c>
       <c r="E12" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1109</v>
+        <v>1110</v>
       </c>
       <c r="B13" s="53" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C13" s="57" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D13" s="55" t="s">
         <v>1110</v>
       </c>
-      <c r="C13" s="57" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D13" s="55" t="s">
-        <v>1109</v>
-      </c>
       <c r="E13" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B14" s="53" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C14" s="57" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D14" s="55" t="s">
+        <v>1113</v>
+      </c>
+      <c r="E14" s="58" t="s">
         <v>1112</v>
-      </c>
-      <c r="B14" s="53" t="s">
-        <v>1113</v>
-      </c>
-      <c r="C14" s="57" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D14" s="55" t="s">
-        <v>1112</v>
-      </c>
-      <c r="E14" s="58" t="s">
-        <v>1111</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1114</v>
+        <v>1115</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>1115</v>
+        <v>1116</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="D15" s="55" t="s">
-        <v>1116</v>
+        <v>1117</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1117</v>
+        <v>1118</v>
       </c>
       <c r="B16" s="53" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C16" s="57" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D16" s="55" t="s">
         <v>1118</v>
       </c>
-      <c r="C16" s="57" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D16" s="55" t="s">
-        <v>1117</v>
-      </c>
       <c r="E16" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1119</v>
+        <v>1120</v>
       </c>
       <c r="B17" s="53" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D17" s="55" t="s">
         <v>1120</v>
       </c>
-      <c r="C17" s="57" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D17" s="55" t="s">
-        <v>1119</v>
-      </c>
       <c r="E17" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1121</v>
+        <v>1122</v>
       </c>
       <c r="B18" s="53" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D18" s="55" t="s">
         <v>1122</v>
       </c>
-      <c r="C18" s="57" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D18" s="55" t="s">
-        <v>1121</v>
-      </c>
       <c r="E18" s="56" t="s">
-        <v>1087</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1123</v>
+        <v>1124</v>
       </c>
       <c r="B19" s="59" t="s">
-        <v>1124</v>
+        <v>1125</v>
       </c>
       <c r="C19" s="57" t="s">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="D19" s="55" t="s">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="E19" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>1126</v>
+        <v>1127</v>
       </c>
       <c r="B20" s="53" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>1091</v>
+      </c>
+      <c r="D20" s="55" t="s">
         <v>1127</v>
       </c>
-      <c r="C20" s="54" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D20" s="55" t="s">
-        <v>1126</v>
-      </c>
       <c r="E20" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1128</v>
+        <v>1129</v>
       </c>
       <c r="B21" s="60" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D21" s="55" t="s">
         <v>1129</v>
       </c>
-      <c r="C21" s="54" t="s">
-        <v>1130</v>
-      </c>
-      <c r="D21" s="55" t="s">
-        <v>1128</v>
-      </c>
       <c r="E21" s="56" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1132</v>
+        <v>1133</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>1133</v>
+        <v>1134</v>
       </c>
       <c r="C22" s="54" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="D22" s="55" t="s">
-        <v>1134</v>
+        <v>1135</v>
       </c>
       <c r="E22" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1135</v>
+        <v>1136</v>
       </c>
       <c r="B23" s="53" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C23" s="54" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D23" s="55" t="s">
         <v>1136</v>
       </c>
-      <c r="C23" s="54" t="s">
-        <v>1130</v>
-      </c>
-      <c r="D23" s="55" t="s">
-        <v>1135</v>
-      </c>
       <c r="E23" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1137</v>
+        <v>1138</v>
       </c>
       <c r="B24" s="53" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D24" s="55" t="s">
         <v>1138</v>
       </c>
-      <c r="C24" s="54" t="s">
-        <v>1130</v>
-      </c>
-      <c r="D24" s="55" t="s">
-        <v>1137</v>
-      </c>
       <c r="E24" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1139</v>
+        <v>1140</v>
       </c>
       <c r="B25" s="53" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D25" s="55" t="s">
         <v>1140</v>
       </c>
-      <c r="C25" s="54" t="s">
-        <v>1141</v>
-      </c>
-      <c r="D25" s="55" t="s">
-        <v>1139</v>
-      </c>
       <c r="E25" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1142</v>
+        <v>1143</v>
       </c>
       <c r="B26" s="62" t="s">
-        <v>1143</v>
+        <v>1144</v>
       </c>
       <c r="C26" s="54" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="D26" s="63" t="s">
-        <v>1144</v>
+        <v>1145</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>1145</v>
+        <v>1146</v>
       </c>
       <c r="B27" s="62" t="s">
-        <v>1146</v>
+        <v>1147</v>
       </c>
       <c r="C27" s="64" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="D27" s="63" t="s">
-        <v>1147</v>
+        <v>1148</v>
       </c>
       <c r="E27" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>1148</v>
+        <v>1149</v>
       </c>
       <c r="B28" s="62" t="s">
-        <v>1149</v>
+        <v>1150</v>
       </c>
       <c r="C28" s="64" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="D28" s="63" t="s">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="E28" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>1151</v>
+        <v>1152</v>
       </c>
       <c r="B29" s="62" t="s">
-        <v>1152</v>
+        <v>1153</v>
       </c>
       <c r="C29" s="64" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="D29" s="63" t="s">
-        <v>1153</v>
+        <v>1154</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="B30" s="62" t="s">
-        <v>1155</v>
+        <v>1156</v>
       </c>
       <c r="C30" s="54" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="D30" s="63" t="s">
-        <v>1156</v>
+        <v>1157</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>1157</v>
+        <v>1158</v>
       </c>
       <c r="B31" s="62" t="s">
-        <v>1158</v>
+        <v>1159</v>
       </c>
       <c r="C31" s="64" t="s">
-        <v>1130</v>
+        <v>1131</v>
       </c>
       <c r="D31" s="63" t="s">
-        <v>1159</v>
+        <v>1160</v>
       </c>
       <c r="E31" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>1160</v>
+        <v>1161</v>
       </c>
       <c r="B32" s="53" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C32" s="54" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D32" s="55" t="s">
         <v>1161</v>
       </c>
-      <c r="C32" s="54" t="s">
-        <v>1130</v>
-      </c>
-      <c r="D32" s="55" t="s">
-        <v>1160</v>
-      </c>
       <c r="E32" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>1162</v>
+        <v>1163</v>
       </c>
       <c r="B33" s="59" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C33" s="57" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D33" s="63" t="s">
         <v>1163</v>
       </c>
-      <c r="C33" s="57" t="s">
-        <v>1164</v>
-      </c>
-      <c r="D33" s="63" t="s">
-        <v>1162</v>
-      </c>
       <c r="E33" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B34" s="59" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C34" s="57" t="s">
         <v>1165</v>
       </c>
-      <c r="B34" s="59" t="s">
+      <c r="D34" s="55" t="s">
         <v>1166</v>
       </c>
-      <c r="C34" s="57" t="s">
-        <v>1164</v>
-      </c>
-      <c r="D34" s="55" t="s">
-        <v>1165</v>
-      </c>
       <c r="E34" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
   </sheetData>
@@ -19144,7 +19147,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -19171,274 +19174,274 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>1168</v>
+        <v>1169</v>
       </c>
       <c r="C2" s="54"/>
       <c r="D2" s="55" t="s">
-        <v>1167</v>
+        <v>1168</v>
       </c>
       <c r="E2" s="65" t="s">
-        <v>1131</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>1169</v>
+        <v>1170</v>
       </c>
       <c r="B3" s="53" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C3" s="54" t="s">
+        <v>1172</v>
+      </c>
+      <c r="D3" s="55" t="s">
         <v>1170</v>
       </c>
-      <c r="C3" s="54" t="s">
-        <v>1171</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>1169</v>
-      </c>
       <c r="E3" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>1173</v>
+        <v>1174</v>
       </c>
       <c r="C4" s="54"/>
       <c r="D4" s="55" t="s">
-        <v>1172</v>
+        <v>1173</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>1175</v>
+        <v>1176</v>
       </c>
       <c r="C5" s="54"/>
       <c r="D5" s="55" t="s">
-        <v>1174</v>
+        <v>1175</v>
       </c>
       <c r="E5" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>1177</v>
+        <v>1178</v>
       </c>
       <c r="C6" s="54"/>
       <c r="D6" s="55" t="s">
-        <v>1176</v>
+        <v>1177</v>
       </c>
       <c r="E6" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="B7" s="53" t="s">
-        <v>1179</v>
+        <v>1180</v>
       </c>
       <c r="C7" s="54"/>
       <c r="D7" s="55" t="s">
-        <v>1178</v>
+        <v>1179</v>
       </c>
       <c r="E7" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="B8" s="53" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="C8" s="54"/>
       <c r="D8" s="55" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="B9" s="53" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="C9" s="54"/>
       <c r="D9" s="55" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
       <c r="E9" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="C10" s="54"/>
       <c r="D10" s="55" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
       <c r="E10" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="B11" s="53" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="C11" s="54"/>
       <c r="D11" s="55" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
       <c r="E11" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="B12" s="53" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
       <c r="C12" s="54"/>
       <c r="D12" s="55" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="B13" s="53" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="C13" s="54"/>
       <c r="D13" s="55" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
       <c r="E13" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>1193</v>
+        <v>1194</v>
       </c>
       <c r="C14" s="54"/>
       <c r="D14" s="55" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
       <c r="E14" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="B15" s="53" t="s">
-        <v>1195</v>
+        <v>1196</v>
       </c>
       <c r="C15" s="54"/>
       <c r="D15" s="55" t="s">
-        <v>1194</v>
+        <v>1195</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="B16" s="53" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="C16" s="54"/>
       <c r="D16" s="55" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B17" s="53" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="C17" s="54"/>
       <c r="D17" s="55" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="E17" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="B18" s="53" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="C18" s="54"/>
       <c r="D18" s="55" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="E18" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="C19" s="54"/>
       <c r="D19" s="55" t="s">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="E19" s="58" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
     </row>
   </sheetData>
@@ -19469,7 +19472,7 @@
       <selection pane="bottomRight" activeCell="AQ9" activeCellId="0" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.27"/>

</xml_diff>

<commit_message>
Corrections in post-processing files and HTML template
</commit_message>
<xml_diff>
--- a/SEPIA/SEPIA_config.xlsx
+++ b/SEPIA/SEPIA_config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" state="visible" r:id="rId2"/>
@@ -432,7 +432,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="1289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="1288">
   <si>
     <t xml:space="preserve">Sheet</t>
   </si>
@@ -4423,9 +4423,6 @@
   </si>
   <si>
     <t xml:space="preserve">GB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EU</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.thinkgeoenergy.com/austrian-oil-gas-and-chemicals-company-to-pivot-to-geothermal/</t>
@@ -5563,7 +5560,7 @@
       <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.91"/>
@@ -6165,13 +6162,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -6748,27 +6745,6 @@
       </c>
       <c r="F29" s="0" t="s">
         <v>1247</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <f aca="false">SUM(B2:B29)</f>
-        <v>1721.88</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <f aca="false">SUM(C2:C29)</f>
-        <v>1833.6</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <f aca="false">SUM(D2:D29)</f>
-        <v>1702.6</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <f aca="false">SUM(E2:E29)</f>
-        <v>1665.6</v>
       </c>
     </row>
   </sheetData>
@@ -6813,13 +6789,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -6855,7 +6831,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6875,7 +6851,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6895,7 +6871,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6915,7 +6891,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6935,7 +6911,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6955,7 +6931,7 @@
         <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6975,7 +6951,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6995,7 +6971,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7015,7 +6991,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7035,7 +7011,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7055,7 +7031,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7075,7 +7051,7 @@
         <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7095,7 +7071,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7115,7 +7091,7 @@
         <v>13</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7135,7 +7111,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7155,7 +7131,7 @@
         <v>60</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7175,7 +7151,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7195,7 +7171,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7215,7 +7191,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7235,7 +7211,7 @@
         <v>12</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7255,7 +7231,7 @@
         <v>1000</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7275,7 +7251,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7295,7 +7271,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7315,7 +7291,7 @@
         <v>40</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7335,7 +7311,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7355,7 +7331,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7375,7 +7351,7 @@
         <v>2.4</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7395,28 +7371,7 @@
         <v>600</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>1288</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B30" s="0" t="n">
-        <f aca="false">SUM(B2:B29)</f>
-        <v>1936.26</v>
-      </c>
-      <c r="C30" s="0" t="n">
-        <f aca="false">SUM(C2:C29)</f>
-        <v>1917.4</v>
-      </c>
-      <c r="D30" s="0" t="n">
-        <f aca="false">SUM(D2:D29)</f>
-        <v>1814.4</v>
-      </c>
-      <c r="E30" s="0" t="n">
-        <f aca="false">SUM(E2:E29)</f>
-        <v>1779.4</v>
+        <v>1287</v>
       </c>
     </row>
   </sheetData>
@@ -7473,7 +7428,7 @@
       <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.28"/>
@@ -7661,7 +7616,7 @@
       <selection pane="bottomRight" activeCell="C73" activeCellId="0" sqref="C73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.36"/>
@@ -10307,7 +10262,7 @@
       <selection pane="bottomLeft" activeCell="C263" activeCellId="0" sqref="C263"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -16072,13 +16027,13 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -17617,7 +17572,7 @@
       <selection pane="bottomLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="8.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
@@ -18530,7 +18485,7 @@
       <selection pane="bottomLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -19147,7 +19102,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="78.54"/>
@@ -19472,7 +19427,7 @@
       <selection pane="bottomRight" activeCell="AQ9" activeCellId="0" sqref="AQ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="12.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="1"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.27"/>

</xml_diff>